<commit_message>
Updated sentiment results with corrected Bulgarian and Slovak data
</commit_message>
<xml_diff>
--- a/results/results_sentiment.xlsx
+++ b/results/results_sentiment.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,42 +450,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Basque</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Finnish</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hebrew</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Vietnamese</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Croatian</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Bulgarian</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Basque</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Finnish</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Hebrew</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Slovak</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Vietnamese</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Croatian</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Chinese</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Thai</t>
         </is>
       </c>
     </row>
@@ -496,31 +501,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7152966793685357</v>
+        <v>0.7005379557680813</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9368535655960806</v>
+        <v>0.7925881649731022</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8062057702776265</v>
+        <v>0.7997609085475195</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8132825258573761</v>
+        <v>0.7686790197250448</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7784431137724551</v>
+        <v>0.7561267184698147</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5612411540555253</v>
+        <v>0.8057381948595338</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7719107240065324</v>
+        <v>0.4459055588762701</v>
       </c>
       <c r="I2" t="n">
-        <v>0.819270549809472</v>
+        <v>0.9318589360430365</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4567229178007621</v>
+        <v>0.7101016138673042</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5415421398684998</v>
       </c>
     </row>
     <row r="3">
@@ -533,28 +541,31 @@
         <v>0.8638110928061504</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6293245469522241</v>
+        <v>0.5365183964854475</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5365183964854475</v>
+        <v>0.5293794618341571</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5293794618341571</v>
+        <v>0.5936298736957716</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5936298736957716</v>
+        <v>0.6496430532674354</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5689181768259198</v>
+        <v>0.598572213069742</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6496430532674354</v>
+        <v>0.5848434925864909</v>
       </c>
       <c r="I3" t="n">
-        <v>0.598572213069742</v>
+        <v>0.5502471169686985</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5848434925864909</v>
+        <v>0.6792970895112576</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5420098846787479</v>
       </c>
     </row>
     <row r="4">
@@ -564,31 +575,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6785714285714286</v>
+        <v>0.7180451127819549</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6569548872180451</v>
+        <v>0.8449248120300752</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8656015037593985</v>
+        <v>0.9003759398496241</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9172932330827067</v>
+        <v>0.8214285714285714</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8176691729323309</v>
+        <v>0.8007518796992481</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9238721804511278</v>
+        <v>0.8721804511278195</v>
       </c>
       <c r="H4" t="n">
-        <v>0.793233082706767</v>
+        <v>0.7377819548872181</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8834586466165414</v>
+        <v>0.8355263157894737</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7603383458646616</v>
+        <v>0.9539473684210527</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.3477443609022556</v>
       </c>
     </row>
     <row r="5">
@@ -601,28 +615,31 @@
         <v>0.5217391304347826</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4210526315789473</v>
+        <v>0.7780320366132724</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7780320366132724</v>
+        <v>0.8237986270022883</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8237986270022883</v>
+        <v>0.6773455377574371</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6773455377574371</v>
+        <v>0.7482837528604119</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4553775743707094</v>
+        <v>0.931350114416476</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7482837528604119</v>
+        <v>0.7276887871853547</v>
       </c>
       <c r="I5" t="n">
-        <v>0.931350114416476</v>
+        <v>0.7665903890160183</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7276887871853547</v>
+        <v>0.8306636155606407</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.2700228832951945</v>
       </c>
     </row>
     <row r="6">
@@ -635,28 +652,31 @@
         <v>0.5985096328607779</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4402035623409669</v>
+        <v>0.52453653217012</v>
       </c>
       <c r="D6" t="n">
-        <v>0.52453653217012</v>
+        <v>0.6012359142130135</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6012359142130135</v>
+        <v>0.4596510359869139</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4596510359869139</v>
+        <v>0.6110505270810614</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4325699745547074</v>
+        <v>0.5703380588876772</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6110505270810614</v>
+        <v>0.9320247182842603</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5703380588876772</v>
+        <v>0.6423118865866958</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9320247182842603</v>
+        <v>0.4463831334060342</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.4278444202108324</v>
       </c>
     </row>
     <row r="7">
@@ -669,28 +689,31 @@
         <v>0.6198830409356725</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5628654970760234</v>
+        <v>0.5497076023391813</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5497076023391813</v>
+        <v>0.5730994152046783</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5730994152046783</v>
+        <v>0.5350877192982456</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5350877192982456</v>
+        <v>0.8114035087719298</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5350877192982456</v>
+        <v>0.6213450292397661</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8114035087719298</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6213450292397661</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5263157894736842</v>
+        <v>0.5380116959064327</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5277777777777778</v>
       </c>
     </row>
     <row r="8">
@@ -703,28 +726,31 @@
         <v>0.6288527397260274</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6164383561643836</v>
+        <v>0.4113869863013699</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4113869863013699</v>
+        <v>0.4991438356164384</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4991438356164384</v>
+        <v>0.5539383561643836</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5539383561643836</v>
+        <v>0.584332191780822</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6476883561643836</v>
+        <v>0.5222602739726028</v>
       </c>
       <c r="H8" t="n">
-        <v>0.584332191780822</v>
+        <v>0.5809075342465754</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5222602739726028</v>
+        <v>0.4357876712328767</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5809075342465754</v>
+        <v>0.6648116438356164</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.827054794520548</v>
       </c>
     </row>
     <row r="9">
@@ -737,28 +763,31 @@
         <v>0.4719387755102041</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5637755102040817</v>
+        <v>0.5663265306122449</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5663265306122449</v>
+        <v>0.8112244897959183</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8112244897959183</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5102040816326531</v>
+        <v>0.4260204081632653</v>
       </c>
       <c r="G9" t="n">
-        <v>0.413265306122449</v>
+        <v>0.3418367346938775</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4260204081632653</v>
+        <v>0.7474489795918368</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3418367346938775</v>
+        <v>0.7525510204081632</v>
       </c>
       <c r="J9" t="n">
-        <v>0.7474489795918368</v>
+        <v>0.5586734693877551</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.2653061224489796</v>
       </c>
     </row>
     <row r="10">
@@ -771,29 +800,32 @@
         <v>0.4361233480176211</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5286343612334802</v>
+        <v>0.8237885462555066</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8237885462555066</v>
+        <v>0.8458149779735683</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8458149779735683</v>
+        <v>0.7224669603524229</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7224669603524229</v>
+        <v>0.5330396475770925</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4933920704845815</v>
+        <v>0.7444933920704846</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5330396475770925</v>
+        <v>0.5859030837004405</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7444933920704846</v>
+        <v>0.73568281938326</v>
       </c>
       <c r="J10" t="n">
         <v>0.5859030837004405</v>
       </c>
+      <c r="K10" t="n">
+        <v>0.3524229074889868</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -805,28 +837,31 @@
         <v>0.529377375036539</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3800058462437884</v>
+        <v>0.6533177433498977</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6533177433498977</v>
+        <v>0.6141479099678456</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6141479099678456</v>
+        <v>0.5808243203741597</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5808243203741597</v>
+        <v>0.3992984507453961</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3007892429114294</v>
+        <v>0.4779304296989185</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3992984507453961</v>
+        <v>0.3291435252850044</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4779304296989185</v>
+        <v>0.5591932183572055</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3291435252850044</v>
+        <v>0.3285589009061678</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.2718503361590178</v>
       </c>
     </row>
     <row r="12">
@@ -839,28 +874,31 @@
         <v>0.6229491173416407</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3026998961578401</v>
+        <v>0.8293873312564901</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8293873312564901</v>
+        <v>0.725441329179647</v>
       </c>
       <c r="E12" t="n">
-        <v>0.725441329179647</v>
+        <v>0.6527518172377985</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6527518172377985</v>
+        <v>0.6428868120456905</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2851505711318795</v>
+        <v>0.6004153686396677</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6428868120456905</v>
+        <v>0.3073727933541018</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6004153686396677</v>
+        <v>0.6512980269989616</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3073727933541018</v>
+        <v>0.4199376947040498</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.3325025960539979</v>
       </c>
     </row>
     <row r="13">
@@ -873,28 +911,31 @@
         <v>0.8026018099547512</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4638009049773756</v>
+        <v>0.9445701357466063</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9445701357466063</v>
+        <v>0.8829185520361991</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8829185520361991</v>
+        <v>0.955316742081448</v>
       </c>
       <c r="F13" t="n">
-        <v>0.955316742081448</v>
+        <v>0.5463800904977375</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5356334841628959</v>
+        <v>0.8297511312217195</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5463800904977375</v>
+        <v>0.3003393665158371</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8297511312217195</v>
+        <v>0.8342760180995475</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3003393665158371</v>
+        <v>0.4270361990950226</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.458710407239819</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -929,42 +970,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Basque</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Finnish</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hebrew</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Vietnamese</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Croatian</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Bulgarian</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Basque</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Finnish</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Hebrew</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Slovak</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Vietnamese</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Croatian</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Chinese</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Thai</t>
         </is>
       </c>
     </row>
@@ -975,31 +1021,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6536469440848467</v>
+        <v>0.652555040727187</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9056750003067346</v>
+        <v>0.6060187510463754</v>
       </c>
       <c r="D2" t="n">
-        <v>0.608203125</v>
+        <v>0.7064618999664317</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7131971168529718</v>
+        <v>0.5767068064638915</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5729371736711462</v>
+        <v>0.6203889221570367</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5318934766850163</v>
+        <v>0.6902526089461462</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6259165389602734</v>
+        <v>0.5619531944307298</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6968543315127173</v>
+        <v>0.922714267134868</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5620925594193799</v>
+        <v>0.612712139789485</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5842069837643795</v>
       </c>
     </row>
     <row r="3">
@@ -1012,28 +1061,31 @@
         <v>0.865822689634096</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6344796482128763</v>
+        <v>0.6698525771494581</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6698525771494581</v>
+        <v>0.6271853815179163</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6271853815179163</v>
+        <v>0.6207650163155138</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6207650163155138</v>
+        <v>0.6801293436908732</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5711467038068709</v>
+        <v>0.6545357895529129</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6801293436908732</v>
+        <v>0.5868121653226006</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6545357895529129</v>
+        <v>0.6782864741641337</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5868121653226006</v>
+        <v>0.6842615543794615</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.56114296873613</v>
       </c>
     </row>
     <row r="4">
@@ -1043,31 +1095,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5779448621553884</v>
+        <v>0.6320802005012531</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5697298057979172</v>
+        <v>0.6001304023845008</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5441970938897168</v>
+        <v>0.7962356211792405</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7072181325617349</v>
+        <v>0.6536019280419532</v>
       </c>
       <c r="F4" t="n">
-        <v>0.607827034454625</v>
+        <v>0.6337568150120452</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7433939601921757</v>
+        <v>0.7046186895810955</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5873006212755166</v>
+        <v>0.5042361111111111</v>
       </c>
       <c r="I4" t="n">
-        <v>0.653061224489796</v>
+        <v>0.5588271819581739</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4950694444444445</v>
+        <v>0.8888818458417851</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.5580788721257094</v>
       </c>
     </row>
     <row r="5">
@@ -1080,28 +1135,31 @@
         <v>0.632750284414107</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5889671093883601</v>
+        <v>0.6445984363894811</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6445984363894811</v>
+        <v>0.7463871744693662</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7463871744693662</v>
+        <v>0.6331578038674033</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6331578038674033</v>
+        <v>0.6397695772695773</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5843526628410349</v>
+        <v>0.9202335967021642</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6397695772695773</v>
+        <v>0.564179104477612</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9202335967021642</v>
+        <v>0.6351397849462366</v>
       </c>
       <c r="J5" t="n">
-        <v>0.564179104477612</v>
+        <v>0.7569867291178767</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5601205029689138</v>
       </c>
     </row>
     <row r="6">
@@ -1114,28 +1172,31 @@
         <v>0.6725091299333675</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5689766610580634</v>
+        <v>0.4664891963788227</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4664891963788227</v>
+        <v>0.5731485080105367</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5731485080105367</v>
+        <v>0.5311155290920716</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5311155290920716</v>
+        <v>0.6315888988865251</v>
       </c>
       <c r="G6" t="n">
-        <v>0.55893690930984</v>
+        <v>0.6252244479217559</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6315888988865251</v>
+        <v>0.9266529807682486</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6252244479217559</v>
+        <v>0.6257499358570412</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9266529807682486</v>
+        <v>0.6039412997903564</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5370569392096878</v>
       </c>
     </row>
     <row r="7">
@@ -1148,28 +1209,31 @@
         <v>0.6439179387994751</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6004533202646409</v>
+        <v>0.5803202961805615</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5803202961805615</v>
+        <v>0.5881135255590874</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5881135255590874</v>
+        <v>0.5417532197756544</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5417532197756544</v>
+        <v>0.8114696507523049</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5578111936695594</v>
+        <v>0.6210793596143914</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8114696507523049</v>
+        <v>0.5245530579759483</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6210793596143914</v>
+        <v>0.5858214235177586</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5245530579759483</v>
+        <v>0.6658476658476659</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5637389950290471</v>
       </c>
     </row>
     <row r="8">
@@ -1182,28 +1246,31 @@
         <v>0.6275595793227636</v>
       </c>
       <c r="C8" t="n">
-        <v>0.595433976213846</v>
+        <v>0.525717999504828</v>
       </c>
       <c r="D8" t="n">
-        <v>0.525717999504828</v>
+        <v>0.5904086178902228</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5904086178902228</v>
+        <v>0.5523004759554856</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5523004759554856</v>
+        <v>0.5771530023179933</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6338321672281246</v>
+        <v>0.5987811180321754</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5771530023179933</v>
+        <v>0.5477582846003899</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5987811180321754</v>
+        <v>0.4832628292704338</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5477582846003899</v>
+        <v>0.6666993464052288</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.8254863278063406</v>
       </c>
     </row>
     <row r="9">
@@ -1216,28 +1283,31 @@
         <v>0.5948076252101373</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5780519650084868</v>
+        <v>0.5462264150943397</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5462264150943397</v>
+        <v>0.7579883805374001</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7579883805374001</v>
+        <v>0.6064591896652965</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6064591896652965</v>
+        <v>0.528657616892911</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5782033743730051</v>
+        <v>0.5896029258098223</v>
       </c>
       <c r="H9" t="n">
-        <v>0.528657616892911</v>
+        <v>0.6093971991069617</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5896029258098223</v>
+        <v>0.6474863912904258</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6093971991069617</v>
+        <v>0.6225302959522959</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4674202127659575</v>
       </c>
     </row>
     <row r="10">
@@ -1250,28 +1320,31 @@
         <v>0.5804822565969063</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5179875679875681</v>
+        <v>0.6913992869875223</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6913992869875223</v>
+        <v>0.6860189573459716</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6860189573459716</v>
+        <v>0.5764471057884232</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5764471057884232</v>
+        <v>0.5499144102085278</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5071139791634272</v>
+        <v>0.633757674250632</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5499144102085278</v>
+        <v>0.5180591467356174</v>
       </c>
       <c r="I10" t="n">
-        <v>0.633757674250632</v>
+        <v>0.5578422380188031</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5180591467356174</v>
+        <v>0.566316199376947</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.5614973262032086</v>
       </c>
     </row>
     <row r="11">
@@ -1284,28 +1357,31 @@
         <v>0.53702445187001</v>
       </c>
       <c r="C11" t="n">
-        <v>0.462026350174216</v>
+        <v>0.5618043840067254</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5618043840067254</v>
+        <v>0.5680857467777496</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5680857467777496</v>
+        <v>0.5883350141966193</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5883350141966193</v>
+        <v>0.4514257310710187</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3605202834334036</v>
+        <v>0.4902041061558005</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4514257310710187</v>
+        <v>0.4213478910749987</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4902041061558005</v>
+        <v>0.4952073071403638</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4213478910749987</v>
+        <v>0.4159575682971945</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.3065643895831066</v>
       </c>
     </row>
     <row r="12">
@@ -1318,28 +1394,31 @@
         <v>0.5878673226891276</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5228735784640599</v>
+        <v>0.5451247873928287</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5451247873928287</v>
+        <v>0.5509681349193779</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5509681349193779</v>
+        <v>0.5279401965565161</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5279401965565161</v>
+        <v>0.5307147113376273</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5166232274341519</v>
+        <v>0.5461487711533696</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5307147113376273</v>
+        <v>0.5152045283280782</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5461487711533696</v>
+        <v>0.5127260398878174</v>
       </c>
       <c r="J12" t="n">
-        <v>0.5152045283280782</v>
+        <v>0.5447759211961229</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.5381076898969719</v>
       </c>
     </row>
     <row r="13">
@@ -1352,28 +1431,31 @@
         <v>0.5625075264932563</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5133727154917397</v>
+        <v>0.4796094198736359</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4796094198736359</v>
+        <v>0.5408005938784833</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5408005938784833</v>
+        <v>0.7210925039872408</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7210925039872408</v>
+        <v>0.5126365263351564</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5252427482792528</v>
+        <v>0.5523527842020992</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5126365263351564</v>
+        <v>0.5026881720430108</v>
       </c>
       <c r="I13" t="n">
-        <v>0.5523527842020992</v>
+        <v>0.521235668014963</v>
       </c>
       <c r="J13" t="n">
-        <v>0.5026881720430108</v>
+        <v>0.5226704190118825</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5087511654407956</v>
       </c>
     </row>
   </sheetData>
@@ -1387,7 +1469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1408,42 +1490,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Basque</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Finnish</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hebrew</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Vietnamese</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Croatian</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Bulgarian</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Basque</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Finnish</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Hebrew</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Slovak</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Vietnamese</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Croatian</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Chinese</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Thai</t>
         </is>
       </c>
     </row>
@@ -1454,31 +1541,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7382792101038624</v>
+        <v>0.7286102523959259</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8836992050751407</v>
+        <v>0.5168035451300899</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5168761967390674</v>
+        <v>0.5136005006346384</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5135011508036285</v>
+        <v>0.5392149058214256</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5395547647138464</v>
+        <v>0.6182528204924087</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5515685743573874</v>
+        <v>0.6416614701498808</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6239560567085083</v>
+        <v>0.5832415650581789</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6454132255381699</v>
+        <v>0.8593612485792501</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5910421058739339</v>
+        <v>0.6487983884164112</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.6278099888109043</v>
       </c>
     </row>
     <row r="3">
@@ -1491,28 +1581,31 @@
         <v>0.8638722424874066</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6294836720514156</v>
+        <v>0.5372463233165422</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5372463233165422</v>
+        <v>0.530099227027966</v>
       </c>
       <c r="E3" t="n">
-        <v>0.530099227027966</v>
+        <v>0.5940177899368884</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5940177899368884</v>
+        <v>0.649980458572173</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5687677320363616</v>
+        <v>0.5990659921255284</v>
       </c>
       <c r="H3" t="n">
-        <v>0.649980458572173</v>
+        <v>0.5847157084129465</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5990659921255284</v>
+        <v>0.5509434167100921</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5847157084129465</v>
+        <v>0.6791605147356841</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5415436280470152</v>
       </c>
     </row>
     <row r="4">
@@ -1522,31 +1615,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7540007123294401</v>
+        <v>0.7867340844194628</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7312491556439826</v>
+        <v>0.5703631885978908</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5466207336993233</v>
+        <v>0.6708802762164241</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6794271888778355</v>
+        <v>0.7341335100594815</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7467177578816797</v>
+        <v>0.7157818086612175</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8484273485378824</v>
+        <v>0.7072973171988906</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7114083244292153</v>
+        <v>0.5059890527969367</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7327659260896798</v>
+        <v>0.5387570260916521</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4895361261560001</v>
+        <v>0.9015610809749393</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.5985534637506852</v>
       </c>
     </row>
     <row r="5">
@@ -1559,28 +1655,31 @@
         <v>0.6710960410557185</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5953537390029325</v>
+        <v>0.5621487047898338</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5621487047898338</v>
+        <v>0.699993890518084</v>
       </c>
       <c r="E5" t="n">
-        <v>0.699993890518084</v>
+        <v>0.6884775171065494</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6884775171065494</v>
+        <v>0.6478647360703813</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6023796432062561</v>
+        <v>0.8736864613880744</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6478647360703813</v>
+        <v>0.5486009286412512</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8736864613880744</v>
+        <v>0.5959799608993157</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5486009286412512</v>
+        <v>0.8016862170087977</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5210318914956011</v>
       </c>
     </row>
     <row r="6">
@@ -1593,28 +1692,31 @@
         <v>0.6488357534487941</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5254989998238031</v>
+        <v>0.4730462361244986</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4730462361244986</v>
+        <v>0.566714550749873</v>
       </c>
       <c r="E6" t="n">
-        <v>0.566714550749873</v>
+        <v>0.5215204751096048</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5215204751096048</v>
+        <v>0.6339724096472954</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5197442036420924</v>
+        <v>0.6135219676005099</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6339724096472954</v>
+        <v>0.9329676730615757</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6135219676005099</v>
+        <v>0.5809384036566027</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9329676730615757</v>
+        <v>0.5344294849869926</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5132895950581968</v>
       </c>
     </row>
     <row r="7">
@@ -1627,28 +1729,31 @@
         <v>0.6247786247786248</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5701470701470701</v>
+        <v>0.5404635404635405</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5404635404635405</v>
+        <v>0.5666435666435666</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5666435666435666</v>
+        <v>0.5386925386925387</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5386925386925387</v>
+        <v>0.811003311003311</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5420035420035419</v>
+        <v>0.6203511203511203</v>
       </c>
       <c r="H7" t="n">
-        <v>0.811003311003311</v>
+        <v>0.5228305228305228</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6203511203511203</v>
+        <v>0.5467005467005467</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5228305228305228</v>
+        <v>0.5490875490875491</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5364210364210364</v>
       </c>
     </row>
     <row r="8">
@@ -1661,28 +1766,31 @@
         <v>0.5660008088018276</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5852052998522761</v>
+        <v>0.5012610024742052</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5012610024742052</v>
+        <v>0.5579207571477672</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5579207571477672</v>
+        <v>0.5541172641253901</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5541172641253901</v>
+        <v>0.57929672177293</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6316617083927984</v>
+        <v>0.5735285079882457</v>
       </c>
       <c r="H8" t="n">
-        <v>0.57929672177293</v>
+        <v>0.5380698316159572</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5735285079882457</v>
+        <v>0.4884275329495698</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5380698316159572</v>
+        <v>0.6161078270924333</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.8133223166330172</v>
       </c>
     </row>
     <row r="9">
@@ -1695,28 +1803,31 @@
         <v>0.6037414965986394</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6037414965986394</v>
+        <v>0.5612244897959183</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5612244897959183</v>
+        <v>0.6972789115646258</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6972789115646258</v>
+        <v>0.6258503401360545</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6258503401360545</v>
+        <v>0.532312925170068</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.5476190476190476</v>
       </c>
       <c r="H9" t="n">
-        <v>0.532312925170068</v>
+        <v>0.5187074829931972</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5476190476190476</v>
+        <v>0.5799319727891157</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5187074829931972</v>
+        <v>0.6547619047619048</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4931972789115647</v>
       </c>
     </row>
     <row r="10">
@@ -1729,28 +1840,31 @@
         <v>0.6316220238095238</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5344494047619047</v>
+        <v>0.7556547619047619</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7556547619047619</v>
+        <v>0.593452380952381</v>
       </c>
       <c r="E10" t="n">
-        <v>0.593452380952381</v>
+        <v>0.6139880952380953</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6139880952380953</v>
+        <v>0.5954613095238095</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5136160714285714</v>
+        <v>0.7204613095238095</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5954613095238095</v>
+        <v>0.5332589285714285</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7204613095238095</v>
+        <v>0.5750744047619047</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5332589285714285</v>
+        <v>0.6267113095238095</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.5821428571428571</v>
       </c>
     </row>
     <row r="11">
@@ -1763,28 +1877,31 @@
         <v>0.5427518442088285</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4669109798619512</v>
+        <v>0.5430141448642836</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5430141448642836</v>
+        <v>0.5726147837156162</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5726147837156162</v>
+        <v>0.6020094562647753</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6020094562647753</v>
+        <v>0.4491595309819176</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3923314120353898</v>
+        <v>0.4887202811578389</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4491595309819176</v>
+        <v>0.4571060350893839</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4887202811578389</v>
+        <v>0.4951149220806945</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4571060350893839</v>
+        <v>0.4499594787985167</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.3833716802264444</v>
       </c>
     </row>
     <row r="12">
@@ -1797,28 +1914,31 @@
         <v>0.654357745398773</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5241353527607362</v>
+        <v>0.5008972392638037</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5008972392638037</v>
+        <v>0.5602147239263804</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5602147239263804</v>
+        <v>0.5421108128834355</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5421108128834355</v>
+        <v>0.5478972392638037</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5160153374233128</v>
+        <v>0.5797331288343559</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5478972392638037</v>
+        <v>0.5169336656441718</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5797331288343559</v>
+        <v>0.5185207055214723</v>
       </c>
       <c r="J12" t="n">
-        <v>0.5169336656441718</v>
+        <v>0.5692960122699386</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.5447595858895705</v>
       </c>
     </row>
     <row r="13">
@@ -1831,28 +1951,31 @@
         <v>0.775714392424079</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5857312407147659</v>
+        <v>0.4920447849145551</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4920447849145551</v>
+        <v>0.5948816054844092</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5948816054844092</v>
+        <v>0.794537999950202</v>
       </c>
       <c r="F13" t="n">
-        <v>0.794537999950202</v>
+        <v>0.581515018217733</v>
       </c>
       <c r="G13" t="n">
-        <v>0.66363591092815</v>
+        <v>0.6953903740652518</v>
       </c>
       <c r="H13" t="n">
-        <v>0.581515018217733</v>
+        <v>0.5140762073916688</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6953903740652518</v>
+        <v>0.5695427722492883</v>
       </c>
       <c r="J13" t="n">
-        <v>0.5140762073916688</v>
+        <v>0.6408035721696117</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5560890386514727</v>
       </c>
     </row>
   </sheetData>
@@ -1866,7 +1989,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,42 +2010,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Basque</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Finnish</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hebrew</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Vietnamese</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Croatian</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Bulgarian</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Basque</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Finnish</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Hebrew</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Slovak</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Vietnamese</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Croatian</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Chinese</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Thai</t>
         </is>
       </c>
     </row>
@@ -1933,31 +2061,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6534578611329636</v>
+        <v>0.6480649878884605</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8941252459407357</v>
+        <v>0.4884418709779182</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4916831449215884</v>
+        <v>0.4747735159637625</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4783086393687618</v>
+        <v>0.5381304817717157</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5404352489573633</v>
+        <v>0.6192892042031992</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4964364035087719</v>
+        <v>0.6578040931973675</v>
       </c>
       <c r="H2" t="n">
-        <v>0.624913684676295</v>
+        <v>0.4383533366433769</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6629670728041167</v>
+        <v>0.886302287760932</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4438952804113654</v>
+        <v>0.6190238073438649</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5163254498201096</v>
       </c>
     </row>
     <row r="3">
@@ -1970,28 +2101,31 @@
         <v>0.8636373518335559</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6259090348822878</v>
+        <v>0.424638518855719</v>
       </c>
       <c r="D3" t="n">
-        <v>0.424638518855719</v>
+        <v>0.4189030032339082</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4189030032339082</v>
+        <v>0.5699860102013203</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5699860102013203</v>
+        <v>0.634470802919708</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5652175896651181</v>
+        <v>0.559236847725493</v>
       </c>
       <c r="H3" t="n">
-        <v>0.634470802919708</v>
+        <v>0.5822674651473847</v>
       </c>
       <c r="I3" t="n">
-        <v>0.559236847725493</v>
+        <v>0.4529419338225827</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5822674651473847</v>
+        <v>0.677017048974802</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5018571533532409</v>
       </c>
     </row>
     <row r="4">
@@ -2001,31 +2135,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5413400019158731</v>
+        <v>0.623113797907762</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5235589055447801</v>
+        <v>0.5800713275974654</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5453358314881054</v>
+        <v>0.7101055899982522</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6919959473150963</v>
+        <v>0.6766226453726454</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6277412280701754</v>
+        <v>0.6532177228422962</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7832650566960142</v>
+        <v>0.7059435557289634</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5974770090038037</v>
+        <v>0.5009204666387584</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6805361847202851</v>
+        <v>0.5435099719290504</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4803642736074004</v>
+        <v>0.8950747353019901</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.3384673272293992</v>
       </c>
     </row>
     <row r="5">
@@ -2038,28 +2175,31 @@
         <v>0.5158985503405507</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4207493097359969</v>
+        <v>0.5644950838872735</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5644950838872735</v>
+        <v>0.7175794200344119</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7175794200344119</v>
+        <v>0.6273969123596321</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6273969123596321</v>
+        <v>0.6433976261127597</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4522540551927533</v>
+        <v>0.8941786129407207</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6433976261127597</v>
+        <v>0.5512843743798159</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8941786129407207</v>
+        <v>0.6059861395940881</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5512843743798159</v>
+        <v>0.7738727903334079</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.2519090933483592</v>
       </c>
     </row>
     <row r="6">
@@ -2072,28 +2212,31 @@
         <v>0.5940762113862558</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3859087500762805</v>
+        <v>0.4603131655517892</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4603131655517892</v>
+        <v>0.5663764345111164</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5663764345111164</v>
+        <v>0.4402233378513725</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4402233378513725</v>
+        <v>0.6108399034625633</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3733023363739249</v>
+        <v>0.5677222303832454</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6108399034625633</v>
+        <v>0.9294555025687101</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5677222303832454</v>
+        <v>0.5679967826980651</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9294555025687101</v>
+        <v>0.3881041885734314</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.3710010586757373</v>
       </c>
     </row>
     <row r="7">
@@ -2106,28 +2249,31 @@
         <v>0.6086267605633804</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5307274875807395</v>
+        <v>0.4802790633418527</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4802790633418527</v>
+        <v>0.5420889007088947</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5420889007088947</v>
+        <v>0.52796875</v>
       </c>
       <c r="F7" t="n">
-        <v>0.52796875</v>
+        <v>0.8111512292634693</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5044788088099945</v>
+        <v>0.6202337900091535</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8111512292634693</v>
+        <v>0.5159700866648029</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6202337900091535</v>
+        <v>0.4931554931554932</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5159700866648029</v>
+        <v>0.446596274182481</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.476006270886154</v>
       </c>
     </row>
     <row r="8">
@@ -2140,28 +2286,31 @@
         <v>0.5368825909542522</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5844631081407317</v>
+        <v>0.301932009655593</v>
       </c>
       <c r="D8" t="n">
-        <v>0.301932009655593</v>
+        <v>0.4744869117799749</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4744869117799749</v>
+        <v>0.5493386654817448</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5493386654817448</v>
+        <v>0.5767331781156937</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6324931359893227</v>
+        <v>0.5075304891871061</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5767331781156937</v>
+        <v>0.5290740570285307</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5075304891871061</v>
+        <v>0.4132322190484249</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5290740570285307</v>
+        <v>0.6089358456873942</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.8178916006730577</v>
       </c>
     </row>
     <row r="9">
@@ -2174,28 +2323,31 @@
         <v>0.4711644366816781</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5411752626715494</v>
+        <v>0.5262604145932266</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5262604145932266</v>
+        <v>0.7172378835731275</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7172378835731275</v>
+        <v>0.5069182389937107</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5069182389937107</v>
+        <v>0.4243684042212984</v>
       </c>
       <c r="G9" t="n">
-        <v>0.412714955706097</v>
+        <v>0.3291055271048372</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4243684042212984</v>
+        <v>0.4805027910525682</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3291055271048372</v>
+        <v>0.5851761343180999</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4805027910525682</v>
+        <v>0.5504557356401844</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.2316864026133116</v>
       </c>
     </row>
     <row r="10">
@@ -2208,28 +2360,31 @@
         <v>0.4223918575063613</v>
       </c>
       <c r="C10" t="n">
-        <v>0.457895324182569</v>
+        <v>0.7130940343781598</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7130940343781598</v>
+        <v>0.6134384274801732</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6134384274801732</v>
+        <v>0.5806773200410497</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5806773200410497</v>
+        <v>0.4791774891774893</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4331531062037218</v>
+        <v>0.6430817610062893</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4791774891774893</v>
+        <v>0.4836914440572978</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6430817610062893</v>
+        <v>0.5617760617760618</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4836914440572978</v>
+        <v>0.5183730588660167</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.3491896319700427</v>
       </c>
     </row>
     <row r="11">
@@ -2242,28 +2397,31 @@
         <v>0.5164668555917252</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3774311464223321</v>
+        <v>0.5380269534167714</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5380269534167714</v>
+        <v>0.5690198851055641</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5690198851055641</v>
+        <v>0.569240428080207</v>
       </c>
       <c r="F11" t="n">
-        <v>0.569240428080207</v>
+        <v>0.3987639612183083</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2930909608603887</v>
+        <v>0.4658246674947822</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3987639612183083</v>
+        <v>0.3068139529031908</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4658246674947822</v>
+        <v>0.4950840145322434</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3068139529031908</v>
+        <v>0.3099356244451651</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.2522404371584699</v>
       </c>
     </row>
     <row r="12">
@@ -2276,28 +2434,31 @@
         <v>0.5571916396424818</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3026004415808584</v>
+        <v>0.4575563205522897</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4575563205522897</v>
+        <v>0.553680759632412</v>
       </c>
       <c r="E12" t="n">
-        <v>0.553680759632412</v>
+        <v>0.5200272148411028</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5200272148411028</v>
+        <v>0.5199710117748938</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2851083576587803</v>
+        <v>0.5174017629307777</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5199710117748938</v>
+        <v>0.3069351180409627</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5174017629307777</v>
+        <v>0.5049457447232601</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3069351180409627</v>
+        <v>0.4064436350751809</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.3314616194616195</v>
       </c>
     </row>
     <row r="13">
@@ -2310,28 +2471,31 @@
         <v>0.559846061111884</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3579036892311229</v>
+        <v>0.4857475276323444</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4857475276323444</v>
+        <v>0.549503128450497</v>
       </c>
       <c r="E13" t="n">
-        <v>0.549503128450497</v>
+        <v>0.7517485065487902</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7517485065487902</v>
+        <v>0.3978886935548251</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4031386529656426</v>
+        <v>0.5552305343154175</v>
       </c>
       <c r="H13" t="n">
-        <v>0.3978886935548251</v>
+        <v>0.2574301430905008</v>
       </c>
       <c r="I13" t="n">
-        <v>0.5552305343154175</v>
+        <v>0.5143216897821956</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2574301430905008</v>
+        <v>0.3433998261515444</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.3521639829462024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-evaluated with Korean model and on Korean data after Korean fix
</commit_message>
<xml_diff>
--- a/results/results_sentiment.xlsx
+++ b/results/results_sentiment.xlsx
@@ -498,7 +498,7 @@
         <v>0.6778242677824268</v>
       </c>
       <c r="M2">
-        <v>0.5983263598326359</v>
+        <v>0.5523012552301255</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -539,7 +539,7 @@
         <v>0.5733113673805601</v>
       </c>
       <c r="M3">
-        <v>0.4777594728171334</v>
+        <v>0.6677649643053267</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -580,7 +580,7 @@
         <v>0.7612781954887218</v>
       </c>
       <c r="M4">
-        <v>0.5958646616541353</v>
+        <v>0.7246240601503759</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -621,7 +621,7 @@
         <v>0.7391304347826086</v>
       </c>
       <c r="M5">
-        <v>0.5606407322654462</v>
+        <v>0.5263157894736842</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -662,7 +662,7 @@
         <v>0.5654307524536533</v>
       </c>
       <c r="M6">
-        <v>0.5872410032715376</v>
+        <v>0.5912395492548165</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -703,7 +703,7 @@
         <v>0.5160818713450293</v>
       </c>
       <c r="M7">
-        <v>0.5233918128654971</v>
+        <v>0.5906432748538012</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -744,7 +744,7 @@
         <v>0.4289383561643836</v>
       </c>
       <c r="M8">
-        <v>0.4190924657534247</v>
+        <v>0.5136986301369864</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -826,7 +826,7 @@
         <v>0.8237885462555066</v>
       </c>
       <c r="M10">
-        <v>0.5682819383259912</v>
+        <v>0.6255506607929515</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -834,40 +834,40 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.529377375036539</v>
+        <v>0.6997840172786177</v>
       </c>
       <c r="C11">
-        <v>0.6533177433498977</v>
+        <v>0.5950323974082073</v>
       </c>
       <c r="D11">
-        <v>0.6141479099678456</v>
+        <v>0.5734341252699784</v>
       </c>
       <c r="E11">
-        <v>0.5808243203741597</v>
+        <v>0.5604751619870411</v>
       </c>
       <c r="F11">
-        <v>0.3992984507453961</v>
+        <v>0.6058315334773218</v>
       </c>
       <c r="G11">
-        <v>0.4779304296989185</v>
+        <v>0.642548596112311</v>
       </c>
       <c r="H11">
-        <v>0.3291435252850044</v>
+        <v>0.4870410367170626</v>
       </c>
       <c r="I11">
-        <v>0.5591932183572055</v>
+        <v>0.6058315334773218</v>
       </c>
       <c r="J11">
-        <v>0.3285589009061678</v>
+        <v>0.5043196544276458</v>
       </c>
       <c r="K11">
-        <v>0.2718503361590178</v>
+        <v>0.4892008639308855</v>
       </c>
       <c r="L11">
-        <v>0.6705641625255773</v>
+        <v>0.6144708423326134</v>
       </c>
       <c r="M11">
-        <v>0.7401344636071324</v>
+        <v>0.7505399568034558</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -908,7 +908,7 @@
         <v>0.8496365524402908</v>
       </c>
       <c r="M12">
-        <v>0.6447559709241952</v>
+        <v>0.7037383177570093</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -949,7 +949,7 @@
         <v>0.8778280542986425</v>
       </c>
       <c r="M13">
-        <v>0.6606334841628959</v>
+        <v>0.6014890282131662</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1044,7 @@
         <v>0.5420116260245246</v>
       </c>
       <c r="M2">
-        <v>0.4956026486202672</v>
+        <v>0.5415139052263731</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1085,7 +1085,7 @@
         <v>0.6310486977962706</v>
       </c>
       <c r="M3">
-        <v>0.4751704808925016</v>
+        <v>0.6959676126342793</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1126,7 +1126,7 @@
         <v>0.5656575288041319</v>
       </c>
       <c r="M4">
-        <v>0.4634044984676121</v>
+        <v>0.624845373577437</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1167,7 +1167,7 @@
         <v>0.6093553302855629</v>
       </c>
       <c r="M5">
-        <v>0.4472835645886262</v>
+        <v>0.5840190700104493</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1208,7 +1208,7 @@
         <v>0.5160115499254844</v>
       </c>
       <c r="M6">
-        <v>0.5158040818038145</v>
+        <v>0.6350509246071655</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1249,7 +1249,7 @@
         <v>0.5132562559391827</v>
       </c>
       <c r="M7">
-        <v>0.5218397884519397</v>
+        <v>0.6009005621635501</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1290,7 +1290,7 @@
         <v>0.4764577684147344</v>
       </c>
       <c r="M8">
-        <v>0.4381302123856752</v>
+        <v>0.5400789715637987</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1331,7 +1331,7 @@
         <v>0.5370138834622697</v>
       </c>
       <c r="M9">
-        <v>0.4409638554216868</v>
+        <v>0.6304415909802693</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1372,7 +1372,7 @@
         <v>0.6074229691876751</v>
       </c>
       <c r="M10">
-        <v>0.4933235629376323</v>
+        <v>0.5622785829307568</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1380,40 +1380,40 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.53702445187001</v>
+        <v>0.7050394725143079</v>
       </c>
       <c r="C11">
-        <v>0.5618043840067254</v>
+        <v>0.5716264521894548</v>
       </c>
       <c r="D11">
-        <v>0.5680857467777496</v>
+        <v>0.5512988661364021</v>
       </c>
       <c r="E11">
-        <v>0.5883350141966193</v>
+        <v>0.559247853676745</v>
       </c>
       <c r="F11">
-        <v>0.4514257310710187</v>
+        <v>0.647521959951709</v>
       </c>
       <c r="G11">
-        <v>0.4902041061558005</v>
+        <v>0.6453601315002988</v>
       </c>
       <c r="H11">
-        <v>0.4213478910749987</v>
+        <v>0.5974310776942355</v>
       </c>
       <c r="I11">
-        <v>0.4952073071403638</v>
+        <v>0.5891006128912838</v>
       </c>
       <c r="J11">
-        <v>0.4159575682971945</v>
+        <v>0.6031447784810127</v>
       </c>
       <c r="K11">
-        <v>0.3065643895831066</v>
+        <v>0.6019638941102756</v>
       </c>
       <c r="L11">
-        <v>0.5768772206459007</v>
+        <v>0.6114594692838967</v>
       </c>
       <c r="M11">
-        <v>0.6994499363441886</v>
+        <v>0.7455492957746479</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1454,7 +1454,7 @@
         <v>0.7323922670754557</v>
       </c>
       <c r="M12">
-        <v>0.4819241516966068</v>
+        <v>0.5667899878492364</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1495,7 +1495,7 @@
         <v>0.5052429781197942</v>
       </c>
       <c r="M13">
-        <v>0.4998826487845767</v>
+        <v>0.4094746437944967</v>
       </c>
     </row>
   </sheetData>
@@ -1590,7 +1590,7 @@
         <v>0.5493503248375812</v>
       </c>
       <c r="M2">
-        <v>0.4939996815751416</v>
+        <v>0.5641493412585743</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1631,7 +1631,7 @@
         <v>0.5738557408372416</v>
       </c>
       <c r="M3">
-        <v>0.4780394157836836</v>
+        <v>0.6680761826182618</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1672,7 +1672,7 @@
         <v>0.601408900125181</v>
       </c>
       <c r="M4">
-        <v>0.4250672950263044</v>
+        <v>0.7642383184834278</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1713,7 +1713,7 @@
         <v>0.6008369990224829</v>
       </c>
       <c r="M5">
-        <v>0.4340786901270772</v>
+        <v>0.6178977272727273</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1754,7 +1754,7 @@
         <v>0.512352849724822</v>
       </c>
       <c r="M6">
-        <v>0.5066664593762632</v>
+        <v>0.6284168195433393</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1795,7 +1795,7 @@
         <v>0.5071610071610072</v>
       </c>
       <c r="M7">
-        <v>0.5175945175945176</v>
+        <v>0.5941325941325941</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1836,7 +1836,7 @@
         <v>0.4847636454959374</v>
       </c>
       <c r="M8">
-        <v>0.439908148640477</v>
+        <v>0.5387295438008679</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1877,7 +1877,7 @@
         <v>0.5493197278911565</v>
       </c>
       <c r="M9">
-        <v>0.4591836734693878</v>
+        <v>0.6734693877551021</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1918,7 +1918,7 @@
         <v>0.5570684523809524</v>
       </c>
       <c r="M10">
-        <v>0.487797619047619</v>
+        <v>0.6151041666666667</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1926,40 +1926,40 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.5427518442088285</v>
+        <v>0.7100525904512616</v>
       </c>
       <c r="C11">
-        <v>0.5430141448642836</v>
+        <v>0.54610892982986</v>
       </c>
       <c r="D11">
-        <v>0.5726147837156162</v>
+        <v>0.5465020398575215</v>
       </c>
       <c r="E11">
-        <v>0.6020094562647753</v>
+        <v>0.560874525990805</v>
       </c>
       <c r="F11">
-        <v>0.4491595309819176</v>
+        <v>0.6359058070021526</v>
       </c>
       <c r="G11">
-        <v>0.4887202811578389</v>
+        <v>0.649228401720096</v>
       </c>
       <c r="H11">
-        <v>0.4571060350893839</v>
+        <v>0.5477101340888717</v>
       </c>
       <c r="I11">
-        <v>0.4951149220806945</v>
+        <v>0.5830756545042259</v>
       </c>
       <c r="J11">
-        <v>0.4499594787985167</v>
+        <v>0.5600020134903856</v>
       </c>
       <c r="K11">
-        <v>0.3833716802264444</v>
+        <v>0.5499297675377409</v>
       </c>
       <c r="L11">
-        <v>0.5409382733619552</v>
+        <v>0.5587987132837631</v>
       </c>
       <c r="M11">
-        <v>0.6995491275093495</v>
+        <v>0.7507370813018653</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2000,7 +2000,7 @@
         <v>0.7285118865030675</v>
       </c>
       <c r="M12">
-        <v>0.4752592024539878</v>
+        <v>0.5940479294478528</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2041,7 +2041,7 @@
         <v>0.5112584760181597</v>
       </c>
       <c r="M13">
-        <v>0.4993318781279308</v>
+        <v>0.4332695954044552</v>
       </c>
     </row>
   </sheetData>
@@ -2136,7 +2136,7 @@
         <v>0.5432955256233967</v>
       </c>
       <c r="M2">
-        <v>0.4849251204011171</v>
+        <v>0.5027758323429803</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2177,7 +2177,7 @@
         <v>0.521347302016447</v>
       </c>
       <c r="M3">
-        <v>0.4623794345979746</v>
+        <v>0.6556178547749867</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2218,7 +2218,7 @@
         <v>0.5715879980723869</v>
       </c>
       <c r="M4">
-        <v>0.4233222246310684</v>
+        <v>0.6206690539723331</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2259,7 +2259,7 @@
         <v>0.604443244616655</v>
       </c>
       <c r="M5">
-        <v>0.4366741862713503</v>
+        <v>0.5098906100157665</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2300,7 +2300,7 @@
         <v>0.5004028402334685</v>
       </c>
       <c r="M6">
-        <v>0.4561841017142525</v>
+        <v>0.5903734094235649</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2341,7 +2341,7 @@
         <v>0.447491916295528</v>
       </c>
       <c r="M7">
-        <v>0.4958033356246156</v>
+        <v>0.584965847231372</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2382,7 +2382,7 @@
         <v>0.4015198306246178</v>
       </c>
       <c r="M8">
-        <v>0.4184930450164742</v>
+        <v>0.5130386273970089</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2423,7 +2423,7 @@
         <v>0.5095033378770403</v>
       </c>
       <c r="M9">
-        <v>0.4451409390544748</v>
+        <v>0.6135211267605634</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2464,7 +2464,7 @@
         <v>0.5656333716035209</v>
       </c>
       <c r="M10">
-        <v>0.4563538611925708</v>
+        <v>0.5353849117484167</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2472,40 +2472,40 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.5164668555917252</v>
+        <v>0.6989061681263566</v>
       </c>
       <c r="C11">
-        <v>0.5380269534167714</v>
+        <v>0.5233977724250098</v>
       </c>
       <c r="D11">
-        <v>0.5690198851055641</v>
+        <v>0.5440703719908108</v>
       </c>
       <c r="E11">
-        <v>0.569240428080207</v>
+        <v>0.5569154007761699</v>
       </c>
       <c r="F11">
-        <v>0.3987639612183083</v>
+        <v>0.6033665553009047</v>
       </c>
       <c r="G11">
-        <v>0.4658246674947822</v>
+        <v>0.64099068233861</v>
       </c>
       <c r="H11">
-        <v>0.3068139529031908</v>
+        <v>0.4435060950537389</v>
       </c>
       <c r="I11">
-        <v>0.4950840145322434</v>
+        <v>0.5829276629560938</v>
       </c>
       <c r="J11">
-        <v>0.3099356244451651</v>
+        <v>0.4720304086157744</v>
       </c>
       <c r="K11">
-        <v>0.2522404371584699</v>
+        <v>0.4458492272850917</v>
       </c>
       <c r="L11">
-        <v>0.5267185065020756</v>
+        <v>0.5265733414485697</v>
       </c>
       <c r="M11">
-        <v>0.6994994504814254</v>
+        <v>0.7467689980075931</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2546,7 +2546,7 @@
         <v>0.7304194179433181</v>
       </c>
       <c r="M12">
-        <v>0.4732452456853908</v>
+        <v>0.5692436357058248</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2587,7 +2587,7 @@
         <v>0.5017951072889705</v>
       </c>
       <c r="M13">
-        <v>0.4317974867965763</v>
+        <v>0.4003967869618839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-evaluated with Hebrew model and on Hebrew data after Hebrew fix
</commit_message>
<xml_diff>
--- a/results/results_sentiment.xlsx
+++ b/results/results_sentiment.xlsx
@@ -31,9 +31,6 @@
     <t>Finnish</t>
   </si>
   <si>
-    <t>Hebrew</t>
-  </si>
-  <si>
     <t>Vietnamese</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>Korean</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0.7005379557680813</v>
@@ -474,31 +474,31 @@
         <v>0.7997609085475195</v>
       </c>
       <c r="E2">
-        <v>0.7686790197250448</v>
+        <v>0.7561267184698147</v>
       </c>
       <c r="F2">
-        <v>0.7561267184698147</v>
+        <v>0.8057381948595338</v>
       </c>
       <c r="G2">
-        <v>0.8057381948595338</v>
+        <v>0.4459055588762701</v>
       </c>
       <c r="H2">
-        <v>0.4459055588762701</v>
+        <v>0.9318589360430365</v>
       </c>
       <c r="I2">
-        <v>0.9318589360430365</v>
+        <v>0.7101016138673042</v>
       </c>
       <c r="J2">
-        <v>0.7101016138673042</v>
+        <v>0.5415421398684998</v>
       </c>
       <c r="K2">
-        <v>0.5415421398684998</v>
+        <v>0.6778242677824268</v>
       </c>
       <c r="L2">
-        <v>0.6778242677824268</v>
+        <v>0.5523012552301255</v>
       </c>
       <c r="M2">
-        <v>0.5523012552301255</v>
+        <v>0.7489539748953975</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -515,36 +515,36 @@
         <v>0.5293794618341571</v>
       </c>
       <c r="E3">
-        <v>0.5936298736957716</v>
+        <v>0.6496430532674354</v>
       </c>
       <c r="F3">
-        <v>0.6496430532674354</v>
+        <v>0.598572213069742</v>
       </c>
       <c r="G3">
-        <v>0.598572213069742</v>
+        <v>0.5848434925864909</v>
       </c>
       <c r="H3">
-        <v>0.5848434925864909</v>
+        <v>0.5502471169686985</v>
       </c>
       <c r="I3">
-        <v>0.5502471169686985</v>
+        <v>0.6792970895112576</v>
       </c>
       <c r="J3">
-        <v>0.6792970895112576</v>
+        <v>0.5420098846787479</v>
       </c>
       <c r="K3">
-        <v>0.5420098846787479</v>
+        <v>0.5733113673805601</v>
       </c>
       <c r="L3">
-        <v>0.5733113673805601</v>
+        <v>0.6677649643053267</v>
       </c>
       <c r="M3">
-        <v>0.6677649643053267</v>
+        <v>0.5826468973091707</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.7180451127819549</v>
@@ -556,36 +556,36 @@
         <v>0.9003759398496241</v>
       </c>
       <c r="E4">
-        <v>0.8214285714285714</v>
+        <v>0.8007518796992481</v>
       </c>
       <c r="F4">
-        <v>0.8007518796992481</v>
+        <v>0.8721804511278195</v>
       </c>
       <c r="G4">
-        <v>0.8721804511278195</v>
+        <v>0.7377819548872181</v>
       </c>
       <c r="H4">
-        <v>0.7377819548872181</v>
+        <v>0.8355263157894737</v>
       </c>
       <c r="I4">
-        <v>0.8355263157894737</v>
+        <v>0.9539473684210527</v>
       </c>
       <c r="J4">
-        <v>0.9539473684210527</v>
+        <v>0.3477443609022556</v>
       </c>
       <c r="K4">
-        <v>0.3477443609022556</v>
+        <v>0.7612781954887218</v>
       </c>
       <c r="L4">
-        <v>0.7612781954887218</v>
+        <v>0.7246240601503759</v>
       </c>
       <c r="M4">
-        <v>0.7246240601503759</v>
+        <v>0.8909774436090225</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0.5217391304347826</v>
@@ -597,36 +597,36 @@
         <v>0.8237986270022883</v>
       </c>
       <c r="E5">
-        <v>0.6773455377574371</v>
+        <v>0.7482837528604119</v>
       </c>
       <c r="F5">
-        <v>0.7482837528604119</v>
+        <v>0.931350114416476</v>
       </c>
       <c r="G5">
-        <v>0.931350114416476</v>
+        <v>0.7276887871853547</v>
       </c>
       <c r="H5">
-        <v>0.7276887871853547</v>
+        <v>0.7665903890160183</v>
       </c>
       <c r="I5">
-        <v>0.7665903890160183</v>
+        <v>0.8306636155606407</v>
       </c>
       <c r="J5">
-        <v>0.8306636155606407</v>
+        <v>0.2700228832951945</v>
       </c>
       <c r="K5">
-        <v>0.2700228832951945</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="L5">
-        <v>0.7391304347826086</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="M5">
-        <v>0.5263157894736842</v>
+        <v>0.7368421052631579</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>0.5985096328607779</v>
@@ -638,36 +638,36 @@
         <v>0.6012359142130135</v>
       </c>
       <c r="E6">
-        <v>0.4596510359869139</v>
+        <v>0.6110505270810614</v>
       </c>
       <c r="F6">
-        <v>0.6110505270810614</v>
+        <v>0.5703380588876772</v>
       </c>
       <c r="G6">
-        <v>0.5703380588876772</v>
+        <v>0.9320247182842603</v>
       </c>
       <c r="H6">
-        <v>0.9320247182842603</v>
+        <v>0.6423118865866958</v>
       </c>
       <c r="I6">
-        <v>0.6423118865866958</v>
+        <v>0.4463831334060342</v>
       </c>
       <c r="J6">
-        <v>0.4463831334060342</v>
+        <v>0.4278444202108324</v>
       </c>
       <c r="K6">
-        <v>0.4278444202108324</v>
+        <v>0.5654307524536533</v>
       </c>
       <c r="L6">
-        <v>0.5654307524536533</v>
+        <v>0.5912395492548165</v>
       </c>
       <c r="M6">
-        <v>0.5912395492548165</v>
+        <v>0.6168665939658307</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0.6198830409356725</v>
@@ -679,36 +679,36 @@
         <v>0.5730994152046783</v>
       </c>
       <c r="E7">
-        <v>0.5350877192982456</v>
+        <v>0.8114035087719298</v>
       </c>
       <c r="F7">
-        <v>0.8114035087719298</v>
+        <v>0.6213450292397661</v>
       </c>
       <c r="G7">
-        <v>0.6213450292397661</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="H7">
-        <v>0.5263157894736842</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I7">
-        <v>0.5555555555555556</v>
+        <v>0.5380116959064327</v>
       </c>
       <c r="J7">
-        <v>0.5380116959064327</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="K7">
-        <v>0.5277777777777778</v>
+        <v>0.5160818713450293</v>
       </c>
       <c r="L7">
-        <v>0.5160818713450293</v>
+        <v>0.5906432748538012</v>
       </c>
       <c r="M7">
-        <v>0.5906432748538012</v>
+        <v>0.5877192982456141</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0.6288527397260274</v>
@@ -720,31 +720,31 @@
         <v>0.4991438356164384</v>
       </c>
       <c r="E8">
-        <v>0.5539383561643836</v>
+        <v>0.584332191780822</v>
       </c>
       <c r="F8">
-        <v>0.584332191780822</v>
+        <v>0.5222602739726028</v>
       </c>
       <c r="G8">
-        <v>0.5222602739726028</v>
+        <v>0.5809075342465754</v>
       </c>
       <c r="H8">
-        <v>0.5809075342465754</v>
+        <v>0.4357876712328767</v>
       </c>
       <c r="I8">
-        <v>0.4357876712328767</v>
+        <v>0.6648116438356164</v>
       </c>
       <c r="J8">
-        <v>0.6648116438356164</v>
+        <v>0.827054794520548</v>
       </c>
       <c r="K8">
-        <v>0.827054794520548</v>
+        <v>0.4289383561643836</v>
       </c>
       <c r="L8">
-        <v>0.4289383561643836</v>
+        <v>0.5136986301369864</v>
       </c>
       <c r="M8">
-        <v>0.5136986301369864</v>
+        <v>0.6228595890410958</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -761,28 +761,28 @@
         <v>0.8112244897959183</v>
       </c>
       <c r="E9">
-        <v>0.5102040816326531</v>
+        <v>0.4260204081632653</v>
       </c>
       <c r="F9">
-        <v>0.4260204081632653</v>
+        <v>0.3418367346938775</v>
       </c>
       <c r="G9">
-        <v>0.3418367346938775</v>
+        <v>0.7474489795918368</v>
       </c>
       <c r="H9">
-        <v>0.7474489795918368</v>
+        <v>0.7525510204081632</v>
       </c>
       <c r="I9">
-        <v>0.7525510204081632</v>
+        <v>0.5586734693877551</v>
       </c>
       <c r="J9">
-        <v>0.5586734693877551</v>
+        <v>0.2653061224489796</v>
       </c>
       <c r="K9">
-        <v>0.2653061224489796</v>
+        <v>0.5433673469387755</v>
       </c>
       <c r="L9">
-        <v>0.5433673469387755</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="M9">
         <v>0.6428571428571429</v>
@@ -802,36 +802,36 @@
         <v>0.8458149779735683</v>
       </c>
       <c r="E10">
-        <v>0.7224669603524229</v>
+        <v>0.5330396475770925</v>
       </c>
       <c r="F10">
-        <v>0.5330396475770925</v>
+        <v>0.7444933920704846</v>
       </c>
       <c r="G10">
-        <v>0.7444933920704846</v>
+        <v>0.5859030837004405</v>
       </c>
       <c r="H10">
+        <v>0.73568281938326</v>
+      </c>
+      <c r="I10">
         <v>0.5859030837004405</v>
       </c>
-      <c r="I10">
+      <c r="J10">
+        <v>0.3524229074889868</v>
+      </c>
+      <c r="K10">
+        <v>0.8237885462555066</v>
+      </c>
+      <c r="L10">
+        <v>0.6255506607929515</v>
+      </c>
+      <c r="M10">
         <v>0.73568281938326</v>
-      </c>
-      <c r="J10">
-        <v>0.5859030837004405</v>
-      </c>
-      <c r="K10">
-        <v>0.3524229074889868</v>
-      </c>
-      <c r="L10">
-        <v>0.8237885462555066</v>
-      </c>
-      <c r="M10">
-        <v>0.6255506607929515</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.6997840172786177</v>
@@ -843,36 +843,36 @@
         <v>0.5734341252699784</v>
       </c>
       <c r="E11">
-        <v>0.5604751619870411</v>
+        <v>0.6058315334773218</v>
       </c>
       <c r="F11">
+        <v>0.642548596112311</v>
+      </c>
+      <c r="G11">
+        <v>0.4870410367170626</v>
+      </c>
+      <c r="H11">
         <v>0.6058315334773218</v>
       </c>
-      <c r="G11">
-        <v>0.642548596112311</v>
-      </c>
-      <c r="H11">
-        <v>0.4870410367170626</v>
-      </c>
       <c r="I11">
-        <v>0.6058315334773218</v>
+        <v>0.5043196544276458</v>
       </c>
       <c r="J11">
-        <v>0.5043196544276458</v>
+        <v>0.4892008639308855</v>
       </c>
       <c r="K11">
-        <v>0.4892008639308855</v>
+        <v>0.6144708423326134</v>
       </c>
       <c r="L11">
-        <v>0.6144708423326134</v>
+        <v>0.7505399568034558</v>
       </c>
       <c r="M11">
-        <v>0.7505399568034558</v>
+        <v>0.6274298056155507</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.6229491173416407</v>
@@ -884,72 +884,72 @@
         <v>0.725441329179647</v>
       </c>
       <c r="E12">
-        <v>0.6527518172377985</v>
+        <v>0.6428868120456905</v>
       </c>
       <c r="F12">
-        <v>0.6428868120456905</v>
+        <v>0.6004153686396677</v>
       </c>
       <c r="G12">
-        <v>0.6004153686396677</v>
+        <v>0.3073727933541018</v>
       </c>
       <c r="H12">
-        <v>0.3073727933541018</v>
+        <v>0.6512980269989616</v>
       </c>
       <c r="I12">
-        <v>0.6512980269989616</v>
+        <v>0.4199376947040498</v>
       </c>
       <c r="J12">
-        <v>0.4199376947040498</v>
+        <v>0.3325025960539979</v>
       </c>
       <c r="K12">
-        <v>0.3325025960539979</v>
+        <v>0.8496365524402908</v>
       </c>
       <c r="L12">
-        <v>0.8496365524402908</v>
+        <v>0.7037383177570093</v>
       </c>
       <c r="M12">
-        <v>0.7037383177570093</v>
+        <v>0.4749740394600208</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.8026018099547512</v>
+        <v>0.717049576783555</v>
       </c>
       <c r="C13">
-        <v>0.9445701357466063</v>
+        <v>0.6783555018137848</v>
       </c>
       <c r="D13">
-        <v>0.8829185520361991</v>
+        <v>0.7174526400644902</v>
       </c>
       <c r="E13">
-        <v>0.955316742081448</v>
+        <v>0.6106408706166868</v>
       </c>
       <c r="F13">
-        <v>0.5463800904977375</v>
+        <v>0.7464731962918179</v>
       </c>
       <c r="G13">
-        <v>0.8297511312217195</v>
+        <v>0.4651350261991133</v>
       </c>
       <c r="H13">
-        <v>0.3003393665158371</v>
+        <v>0.6723095525997581</v>
       </c>
       <c r="I13">
-        <v>0.8342760180995475</v>
+        <v>0.5578395808141878</v>
       </c>
       <c r="J13">
-        <v>0.4270361990950226</v>
+        <v>0.5808141878274889</v>
       </c>
       <c r="K13">
-        <v>0.458710407239819</v>
+        <v>0.6444981862152358</v>
       </c>
       <c r="L13">
-        <v>0.8778280542986425</v>
+        <v>0.6187021362353889</v>
       </c>
       <c r="M13">
-        <v>0.6014890282131662</v>
+        <v>0.9286577992744861</v>
       </c>
     </row>
   </sheetData>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0.652555040727187</v>
@@ -1020,31 +1020,31 @@
         <v>0.7064618999664317</v>
       </c>
       <c r="E2">
-        <v>0.5767068064638915</v>
+        <v>0.6203889221570367</v>
       </c>
       <c r="F2">
-        <v>0.6203889221570367</v>
+        <v>0.6902526089461462</v>
       </c>
       <c r="G2">
-        <v>0.6902526089461462</v>
+        <v>0.5619531944307298</v>
       </c>
       <c r="H2">
-        <v>0.5619531944307298</v>
+        <v>0.922714267134868</v>
       </c>
       <c r="I2">
-        <v>0.922714267134868</v>
+        <v>0.612712139789485</v>
       </c>
       <c r="J2">
-        <v>0.612712139789485</v>
+        <v>0.5842069837643795</v>
       </c>
       <c r="K2">
-        <v>0.5842069837643795</v>
+        <v>0.5420116260245246</v>
       </c>
       <c r="L2">
-        <v>0.5420116260245246</v>
+        <v>0.5415139052263731</v>
       </c>
       <c r="M2">
-        <v>0.5415139052263731</v>
+        <v>0.5481625933541061</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1061,36 +1061,36 @@
         <v>0.6271853815179163</v>
       </c>
       <c r="E3">
-        <v>0.6207650163155138</v>
+        <v>0.6801293436908732</v>
       </c>
       <c r="F3">
-        <v>0.6801293436908732</v>
+        <v>0.6545357895529129</v>
       </c>
       <c r="G3">
-        <v>0.6545357895529129</v>
+        <v>0.5868121653226006</v>
       </c>
       <c r="H3">
-        <v>0.5868121653226006</v>
+        <v>0.6782864741641337</v>
       </c>
       <c r="I3">
-        <v>0.6782864741641337</v>
+        <v>0.6842615543794615</v>
       </c>
       <c r="J3">
-        <v>0.6842615543794615</v>
+        <v>0.56114296873613</v>
       </c>
       <c r="K3">
-        <v>0.56114296873613</v>
+        <v>0.6310486977962706</v>
       </c>
       <c r="L3">
-        <v>0.6310486977962706</v>
+        <v>0.6959676126342793</v>
       </c>
       <c r="M3">
-        <v>0.6959676126342793</v>
+        <v>0.6408034241092578</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.6320802005012531</v>
@@ -1102,36 +1102,36 @@
         <v>0.7962356211792405</v>
       </c>
       <c r="E4">
-        <v>0.6536019280419532</v>
+        <v>0.6337568150120452</v>
       </c>
       <c r="F4">
-        <v>0.6337568150120452</v>
+        <v>0.7046186895810955</v>
       </c>
       <c r="G4">
-        <v>0.7046186895810955</v>
+        <v>0.5042361111111111</v>
       </c>
       <c r="H4">
-        <v>0.5042361111111111</v>
+        <v>0.5588271819581739</v>
       </c>
       <c r="I4">
-        <v>0.5588271819581739</v>
+        <v>0.8888818458417851</v>
       </c>
       <c r="J4">
-        <v>0.8888818458417851</v>
+        <v>0.5580788721257094</v>
       </c>
       <c r="K4">
-        <v>0.5580788721257094</v>
+        <v>0.5656575288041319</v>
       </c>
       <c r="L4">
-        <v>0.5656575288041319</v>
+        <v>0.624845373577437</v>
       </c>
       <c r="M4">
-        <v>0.624845373577437</v>
+        <v>0.7481069737103315</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0.632750284414107</v>
@@ -1143,36 +1143,36 @@
         <v>0.7463871744693662</v>
       </c>
       <c r="E5">
-        <v>0.6331578038674033</v>
+        <v>0.6397695772695773</v>
       </c>
       <c r="F5">
-        <v>0.6397695772695773</v>
+        <v>0.9202335967021642</v>
       </c>
       <c r="G5">
-        <v>0.9202335967021642</v>
+        <v>0.564179104477612</v>
       </c>
       <c r="H5">
-        <v>0.564179104477612</v>
+        <v>0.6351397849462366</v>
       </c>
       <c r="I5">
-        <v>0.6351397849462366</v>
+        <v>0.7569867291178767</v>
       </c>
       <c r="J5">
-        <v>0.7569867291178767</v>
+        <v>0.5601205029689138</v>
       </c>
       <c r="K5">
-        <v>0.5601205029689138</v>
+        <v>0.6093553302855629</v>
       </c>
       <c r="L5">
-        <v>0.6093553302855629</v>
+        <v>0.5840190700104493</v>
       </c>
       <c r="M5">
-        <v>0.5840190700104493</v>
+        <v>0.6286781159095994</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>0.6725091299333675</v>
@@ -1184,36 +1184,36 @@
         <v>0.5731485080105367</v>
       </c>
       <c r="E6">
-        <v>0.5311155290920716</v>
+        <v>0.6315888988865251</v>
       </c>
       <c r="F6">
-        <v>0.6315888988865251</v>
+        <v>0.6252244479217559</v>
       </c>
       <c r="G6">
-        <v>0.6252244479217559</v>
+        <v>0.9266529807682486</v>
       </c>
       <c r="H6">
-        <v>0.9266529807682486</v>
+        <v>0.6257499358570412</v>
       </c>
       <c r="I6">
-        <v>0.6257499358570412</v>
+        <v>0.6039412997903564</v>
       </c>
       <c r="J6">
-        <v>0.6039412997903564</v>
+        <v>0.5370569392096878</v>
       </c>
       <c r="K6">
-        <v>0.5370569392096878</v>
+        <v>0.5160115499254844</v>
       </c>
       <c r="L6">
-        <v>0.5160115499254844</v>
+        <v>0.6350509246071655</v>
       </c>
       <c r="M6">
-        <v>0.6350509246071655</v>
+        <v>0.6198502424881566</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0.6439179387994751</v>
@@ -1225,36 +1225,36 @@
         <v>0.5881135255590874</v>
       </c>
       <c r="E7">
-        <v>0.5417532197756544</v>
+        <v>0.8114696507523049</v>
       </c>
       <c r="F7">
-        <v>0.8114696507523049</v>
+        <v>0.6210793596143914</v>
       </c>
       <c r="G7">
-        <v>0.6210793596143914</v>
+        <v>0.5245530579759483</v>
       </c>
       <c r="H7">
-        <v>0.5245530579759483</v>
+        <v>0.5858214235177586</v>
       </c>
       <c r="I7">
-        <v>0.5858214235177586</v>
+        <v>0.6658476658476659</v>
       </c>
       <c r="J7">
-        <v>0.6658476658476659</v>
+        <v>0.5637389950290471</v>
       </c>
       <c r="K7">
-        <v>0.5637389950290471</v>
+        <v>0.5132562559391827</v>
       </c>
       <c r="L7">
-        <v>0.5132562559391827</v>
+        <v>0.6009005621635501</v>
       </c>
       <c r="M7">
-        <v>0.6009005621635501</v>
+        <v>0.5898160345219169</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0.6275595793227636</v>
@@ -1266,31 +1266,31 @@
         <v>0.5904086178902228</v>
       </c>
       <c r="E8">
-        <v>0.5523004759554856</v>
+        <v>0.5771530023179933</v>
       </c>
       <c r="F8">
-        <v>0.5771530023179933</v>
+        <v>0.5987811180321754</v>
       </c>
       <c r="G8">
-        <v>0.5987811180321754</v>
+        <v>0.5477582846003899</v>
       </c>
       <c r="H8">
-        <v>0.5477582846003899</v>
+        <v>0.4832628292704338</v>
       </c>
       <c r="I8">
-        <v>0.4832628292704338</v>
+        <v>0.6666993464052288</v>
       </c>
       <c r="J8">
-        <v>0.6666993464052288</v>
+        <v>0.8254863278063406</v>
       </c>
       <c r="K8">
-        <v>0.8254863278063406</v>
+        <v>0.4764577684147344</v>
       </c>
       <c r="L8">
-        <v>0.4764577684147344</v>
+        <v>0.5400789715637987</v>
       </c>
       <c r="M8">
-        <v>0.5400789715637987</v>
+        <v>0.6141441120607787</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1307,31 +1307,31 @@
         <v>0.7579883805374001</v>
       </c>
       <c r="E9">
-        <v>0.6064591896652965</v>
+        <v>0.528657616892911</v>
       </c>
       <c r="F9">
-        <v>0.528657616892911</v>
+        <v>0.5896029258098223</v>
       </c>
       <c r="G9">
-        <v>0.5896029258098223</v>
+        <v>0.6093971991069617</v>
       </c>
       <c r="H9">
-        <v>0.6093971991069617</v>
+        <v>0.6474863912904258</v>
       </c>
       <c r="I9">
-        <v>0.6474863912904258</v>
+        <v>0.6225302959522959</v>
       </c>
       <c r="J9">
-        <v>0.6225302959522959</v>
+        <v>0.4674202127659575</v>
       </c>
       <c r="K9">
-        <v>0.4674202127659575</v>
+        <v>0.5370138834622697</v>
       </c>
       <c r="L9">
-        <v>0.5370138834622697</v>
+        <v>0.6304415909802693</v>
       </c>
       <c r="M9">
-        <v>0.6304415909802693</v>
+        <v>0.6256410256410256</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1348,36 +1348,36 @@
         <v>0.6860189573459716</v>
       </c>
       <c r="E10">
-        <v>0.5764471057884232</v>
+        <v>0.5499144102085278</v>
       </c>
       <c r="F10">
-        <v>0.5499144102085278</v>
+        <v>0.633757674250632</v>
       </c>
       <c r="G10">
-        <v>0.633757674250632</v>
+        <v>0.5180591467356174</v>
       </c>
       <c r="H10">
-        <v>0.5180591467356174</v>
+        <v>0.5578422380188031</v>
       </c>
       <c r="I10">
-        <v>0.5578422380188031</v>
+        <v>0.566316199376947</v>
       </c>
       <c r="J10">
-        <v>0.566316199376947</v>
+        <v>0.5614973262032086</v>
       </c>
       <c r="K10">
-        <v>0.5614973262032086</v>
+        <v>0.6074229691876751</v>
       </c>
       <c r="L10">
-        <v>0.6074229691876751</v>
+        <v>0.5622785829307568</v>
       </c>
       <c r="M10">
-        <v>0.5622785829307568</v>
+        <v>0.5717306441119063</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.7050394725143079</v>
@@ -1389,36 +1389,36 @@
         <v>0.5512988661364021</v>
       </c>
       <c r="E11">
-        <v>0.559247853676745</v>
+        <v>0.647521959951709</v>
       </c>
       <c r="F11">
-        <v>0.647521959951709</v>
+        <v>0.6453601315002988</v>
       </c>
       <c r="G11">
-        <v>0.6453601315002988</v>
+        <v>0.5974310776942355</v>
       </c>
       <c r="H11">
-        <v>0.5974310776942355</v>
+        <v>0.5891006128912838</v>
       </c>
       <c r="I11">
-        <v>0.5891006128912838</v>
+        <v>0.6031447784810127</v>
       </c>
       <c r="J11">
-        <v>0.6031447784810127</v>
+        <v>0.6019638941102756</v>
       </c>
       <c r="K11">
-        <v>0.6019638941102756</v>
+        <v>0.6114594692838967</v>
       </c>
       <c r="L11">
-        <v>0.6114594692838967</v>
+        <v>0.7455492957746479</v>
       </c>
       <c r="M11">
-        <v>0.7455492957746479</v>
+        <v>0.618901976404537</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.5878673226891276</v>
@@ -1430,72 +1430,72 @@
         <v>0.5509681349193779</v>
       </c>
       <c r="E12">
-        <v>0.5279401965565161</v>
+        <v>0.5307147113376273</v>
       </c>
       <c r="F12">
-        <v>0.5307147113376273</v>
+        <v>0.5461487711533696</v>
       </c>
       <c r="G12">
-        <v>0.5461487711533696</v>
+        <v>0.5152045283280782</v>
       </c>
       <c r="H12">
-        <v>0.5152045283280782</v>
+        <v>0.5127260398878174</v>
       </c>
       <c r="I12">
-        <v>0.5127260398878174</v>
+        <v>0.5447759211961229</v>
       </c>
       <c r="J12">
-        <v>0.5447759211961229</v>
+        <v>0.5381076898969719</v>
       </c>
       <c r="K12">
-        <v>0.5381076898969719</v>
+        <v>0.7323922670754557</v>
       </c>
       <c r="L12">
-        <v>0.7323922670754557</v>
+        <v>0.5667899878492364</v>
       </c>
       <c r="M12">
-        <v>0.5667899878492364</v>
+        <v>0.5196306690911008</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.5625075264932563</v>
+        <v>0.6707604416216316</v>
       </c>
       <c r="C13">
-        <v>0.4796094198736359</v>
+        <v>0.5045729209340434</v>
       </c>
       <c r="D13">
-        <v>0.5408005938784833</v>
+        <v>0.6718988555408572</v>
       </c>
       <c r="E13">
-        <v>0.7210925039872408</v>
+        <v>0.630935633107927</v>
       </c>
       <c r="F13">
-        <v>0.5126365263351564</v>
+        <v>0.7052451649767086</v>
       </c>
       <c r="G13">
-        <v>0.5523527842020992</v>
+        <v>0.5862139454465227</v>
       </c>
       <c r="H13">
-        <v>0.5026881720430108</v>
+        <v>0.5931478689129233</v>
       </c>
       <c r="I13">
-        <v>0.521235668014963</v>
+        <v>0.6446745029160755</v>
       </c>
       <c r="J13">
-        <v>0.5226704190118825</v>
+        <v>0.6488247962290792</v>
       </c>
       <c r="K13">
-        <v>0.5087511654407956</v>
+        <v>0.4718507817523435</v>
       </c>
       <c r="L13">
-        <v>0.5052429781197942</v>
+        <v>0.6300606871617893</v>
       </c>
       <c r="M13">
-        <v>0.4094746437944967</v>
+        <v>0.9211556022806627</v>
       </c>
     </row>
   </sheetData>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0.7286102523959259</v>
@@ -1566,31 +1566,31 @@
         <v>0.5136005006346384</v>
       </c>
       <c r="E2">
-        <v>0.5392149058214256</v>
+        <v>0.6182528204924087</v>
       </c>
       <c r="F2">
-        <v>0.6182528204924087</v>
+        <v>0.6416614701498808</v>
       </c>
       <c r="G2">
-        <v>0.6416614701498808</v>
+        <v>0.5832415650581789</v>
       </c>
       <c r="H2">
-        <v>0.5832415650581789</v>
+        <v>0.8593612485792501</v>
       </c>
       <c r="I2">
-        <v>0.8593612485792501</v>
+        <v>0.6487983884164112</v>
       </c>
       <c r="J2">
-        <v>0.6487983884164112</v>
+        <v>0.6278099888109043</v>
       </c>
       <c r="K2">
-        <v>0.6278099888109043</v>
+        <v>0.5493503248375812</v>
       </c>
       <c r="L2">
-        <v>0.5493503248375812</v>
+        <v>0.5641493412585743</v>
       </c>
       <c r="M2">
-        <v>0.5641493412585743</v>
+        <v>0.5301464312091742</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1607,36 +1607,36 @@
         <v>0.530099227027966</v>
       </c>
       <c r="E3">
-        <v>0.5940177899368884</v>
+        <v>0.649980458572173</v>
       </c>
       <c r="F3">
-        <v>0.649980458572173</v>
+        <v>0.5990659921255284</v>
       </c>
       <c r="G3">
-        <v>0.5990659921255284</v>
+        <v>0.5847157084129465</v>
       </c>
       <c r="H3">
-        <v>0.5847157084129465</v>
+        <v>0.5509434167100921</v>
       </c>
       <c r="I3">
-        <v>0.5509434167100921</v>
+        <v>0.6791605147356841</v>
       </c>
       <c r="J3">
-        <v>0.6791605147356841</v>
+        <v>0.5415436280470152</v>
       </c>
       <c r="K3">
-        <v>0.5415436280470152</v>
+        <v>0.5738557408372416</v>
       </c>
       <c r="L3">
-        <v>0.5738557408372416</v>
+        <v>0.6680761826182618</v>
       </c>
       <c r="M3">
-        <v>0.6680761826182618</v>
+        <v>0.5831741068843727</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.7867340844194628</v>
@@ -1648,36 +1648,36 @@
         <v>0.6708802762164241</v>
       </c>
       <c r="E4">
-        <v>0.7341335100594815</v>
+        <v>0.7157818086612175</v>
       </c>
       <c r="F4">
-        <v>0.7157818086612175</v>
+        <v>0.7072973171988906</v>
       </c>
       <c r="G4">
-        <v>0.7072973171988906</v>
+        <v>0.5059890527969367</v>
       </c>
       <c r="H4">
-        <v>0.5059890527969367</v>
+        <v>0.5387570260916521</v>
       </c>
       <c r="I4">
-        <v>0.5387570260916521</v>
+        <v>0.9015610809749393</v>
       </c>
       <c r="J4">
-        <v>0.9015610809749393</v>
+        <v>0.5985534637506852</v>
       </c>
       <c r="K4">
-        <v>0.5985534637506852</v>
+        <v>0.601408900125181</v>
       </c>
       <c r="L4">
-        <v>0.601408900125181</v>
+        <v>0.7642383184834278</v>
       </c>
       <c r="M4">
-        <v>0.7642383184834278</v>
+        <v>0.7147345425983653</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0.6710960410557185</v>
@@ -1689,36 +1689,36 @@
         <v>0.699993890518084</v>
       </c>
       <c r="E5">
-        <v>0.6884775171065494</v>
+        <v>0.6478647360703813</v>
       </c>
       <c r="F5">
-        <v>0.6478647360703813</v>
+        <v>0.8736864613880744</v>
       </c>
       <c r="G5">
-        <v>0.8736864613880744</v>
+        <v>0.5486009286412512</v>
       </c>
       <c r="H5">
-        <v>0.5486009286412512</v>
+        <v>0.5959799608993157</v>
       </c>
       <c r="I5">
-        <v>0.5959799608993157</v>
+        <v>0.8016862170087977</v>
       </c>
       <c r="J5">
-        <v>0.8016862170087977</v>
+        <v>0.5210318914956011</v>
       </c>
       <c r="K5">
-        <v>0.5210318914956011</v>
+        <v>0.6008369990224829</v>
       </c>
       <c r="L5">
-        <v>0.6008369990224829</v>
+        <v>0.6178977272727273</v>
       </c>
       <c r="M5">
-        <v>0.6178977272727273</v>
+        <v>0.640533357771261</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>0.6488357534487941</v>
@@ -1730,36 +1730,36 @@
         <v>0.566714550749873</v>
       </c>
       <c r="E6">
-        <v>0.5215204751096048</v>
+        <v>0.6339724096472954</v>
       </c>
       <c r="F6">
-        <v>0.6339724096472954</v>
+        <v>0.6135219676005099</v>
       </c>
       <c r="G6">
-        <v>0.6135219676005099</v>
+        <v>0.9329676730615757</v>
       </c>
       <c r="H6">
-        <v>0.9329676730615757</v>
+        <v>0.5809384036566027</v>
       </c>
       <c r="I6">
-        <v>0.5809384036566027</v>
+        <v>0.5344294849869926</v>
       </c>
       <c r="J6">
-        <v>0.5344294849869926</v>
+        <v>0.5132895950581968</v>
       </c>
       <c r="K6">
-        <v>0.5132895950581968</v>
+        <v>0.512352849724822</v>
       </c>
       <c r="L6">
-        <v>0.512352849724822</v>
+        <v>0.6284168195433393</v>
       </c>
       <c r="M6">
-        <v>0.6284168195433393</v>
+        <v>0.6252496294684038</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0.6247786247786248</v>
@@ -1771,36 +1771,36 @@
         <v>0.5666435666435666</v>
       </c>
       <c r="E7">
-        <v>0.5386925386925387</v>
+        <v>0.811003311003311</v>
       </c>
       <c r="F7">
-        <v>0.811003311003311</v>
+        <v>0.6203511203511203</v>
       </c>
       <c r="G7">
-        <v>0.6203511203511203</v>
+        <v>0.5228305228305228</v>
       </c>
       <c r="H7">
-        <v>0.5228305228305228</v>
+        <v>0.5467005467005467</v>
       </c>
       <c r="I7">
-        <v>0.5467005467005467</v>
+        <v>0.5490875490875491</v>
       </c>
       <c r="J7">
-        <v>0.5490875490875491</v>
+        <v>0.5364210364210364</v>
       </c>
       <c r="K7">
-        <v>0.5364210364210364</v>
+        <v>0.5071610071610072</v>
       </c>
       <c r="L7">
-        <v>0.5071610071610072</v>
+        <v>0.5941325941325941</v>
       </c>
       <c r="M7">
-        <v>0.5941325941325941</v>
+        <v>0.5845845845845846</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0.5660008088018276</v>
@@ -1812,31 +1812,31 @@
         <v>0.5579207571477672</v>
       </c>
       <c r="E8">
-        <v>0.5541172641253901</v>
+        <v>0.57929672177293</v>
       </c>
       <c r="F8">
-        <v>0.57929672177293</v>
+        <v>0.5735285079882457</v>
       </c>
       <c r="G8">
-        <v>0.5735285079882457</v>
+        <v>0.5380698316159572</v>
       </c>
       <c r="H8">
-        <v>0.5380698316159572</v>
+        <v>0.4884275329495698</v>
       </c>
       <c r="I8">
-        <v>0.4884275329495698</v>
+        <v>0.6161078270924333</v>
       </c>
       <c r="J8">
-        <v>0.6161078270924333</v>
+        <v>0.8133223166330172</v>
       </c>
       <c r="K8">
-        <v>0.8133223166330172</v>
+        <v>0.4847636454959374</v>
       </c>
       <c r="L8">
-        <v>0.4847636454959374</v>
+        <v>0.5387295438008679</v>
       </c>
       <c r="M8">
-        <v>0.5387295438008679</v>
+        <v>0.6167284648926137</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1853,31 +1853,31 @@
         <v>0.6972789115646258</v>
       </c>
       <c r="E9">
-        <v>0.6258503401360545</v>
+        <v>0.532312925170068</v>
       </c>
       <c r="F9">
-        <v>0.532312925170068</v>
+        <v>0.5476190476190476</v>
       </c>
       <c r="G9">
-        <v>0.5476190476190476</v>
+        <v>0.5187074829931972</v>
       </c>
       <c r="H9">
-        <v>0.5187074829931972</v>
+        <v>0.5799319727891157</v>
       </c>
       <c r="I9">
-        <v>0.5799319727891157</v>
+        <v>0.6547619047619048</v>
       </c>
       <c r="J9">
-        <v>0.6547619047619048</v>
+        <v>0.4931972789115647</v>
       </c>
       <c r="K9">
-        <v>0.4931972789115647</v>
+        <v>0.5493197278911565</v>
       </c>
       <c r="L9">
-        <v>0.5493197278911565</v>
+        <v>0.6734693877551021</v>
       </c>
       <c r="M9">
-        <v>0.6734693877551021</v>
+        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1894,36 +1894,36 @@
         <v>0.593452380952381</v>
       </c>
       <c r="E10">
-        <v>0.6139880952380953</v>
+        <v>0.5954613095238095</v>
       </c>
       <c r="F10">
-        <v>0.5954613095238095</v>
+        <v>0.7204613095238095</v>
       </c>
       <c r="G10">
-        <v>0.7204613095238095</v>
+        <v>0.5332589285714285</v>
       </c>
       <c r="H10">
-        <v>0.5332589285714285</v>
+        <v>0.5750744047619047</v>
       </c>
       <c r="I10">
-        <v>0.5750744047619047</v>
+        <v>0.6267113095238095</v>
       </c>
       <c r="J10">
-        <v>0.6267113095238095</v>
+        <v>0.5821428571428571</v>
       </c>
       <c r="K10">
-        <v>0.5821428571428571</v>
+        <v>0.5570684523809524</v>
       </c>
       <c r="L10">
-        <v>0.5570684523809524</v>
+        <v>0.6151041666666667</v>
       </c>
       <c r="M10">
-        <v>0.6151041666666667</v>
+        <v>0.5984375</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.7100525904512616</v>
@@ -1935,36 +1935,36 @@
         <v>0.5465020398575215</v>
       </c>
       <c r="E11">
-        <v>0.560874525990805</v>
+        <v>0.6359058070021526</v>
       </c>
       <c r="F11">
-        <v>0.6359058070021526</v>
+        <v>0.649228401720096</v>
       </c>
       <c r="G11">
-        <v>0.649228401720096</v>
+        <v>0.5477101340888717</v>
       </c>
       <c r="H11">
-        <v>0.5477101340888717</v>
+        <v>0.5830756545042259</v>
       </c>
       <c r="I11">
-        <v>0.5830756545042259</v>
+        <v>0.5600020134903856</v>
       </c>
       <c r="J11">
-        <v>0.5600020134903856</v>
+        <v>0.5499297675377409</v>
       </c>
       <c r="K11">
-        <v>0.5499297675377409</v>
+        <v>0.5587987132837631</v>
       </c>
       <c r="L11">
-        <v>0.5587987132837631</v>
+        <v>0.7507370813018653</v>
       </c>
       <c r="M11">
-        <v>0.7507370813018653</v>
+        <v>0.6202101700440571</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.654357745398773</v>
@@ -1976,72 +1976,72 @@
         <v>0.5602147239263804</v>
       </c>
       <c r="E12">
-        <v>0.5421108128834355</v>
+        <v>0.5478972392638037</v>
       </c>
       <c r="F12">
-        <v>0.5478972392638037</v>
+        <v>0.5797331288343559</v>
       </c>
       <c r="G12">
-        <v>0.5797331288343559</v>
+        <v>0.5169336656441718</v>
       </c>
       <c r="H12">
-        <v>0.5169336656441718</v>
+        <v>0.5185207055214723</v>
       </c>
       <c r="I12">
-        <v>0.5185207055214723</v>
+        <v>0.5692960122699386</v>
       </c>
       <c r="J12">
-        <v>0.5692960122699386</v>
+        <v>0.5447595858895705</v>
       </c>
       <c r="K12">
-        <v>0.5447595858895705</v>
+        <v>0.7285118865030675</v>
       </c>
       <c r="L12">
-        <v>0.7285118865030675</v>
+        <v>0.5940479294478528</v>
       </c>
       <c r="M12">
-        <v>0.5940479294478528</v>
+        <v>0.5342756901840491</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.775714392424079</v>
+        <v>0.6658678129472178</v>
       </c>
       <c r="C13">
-        <v>0.4920447849145551</v>
+        <v>0.5003356012410857</v>
       </c>
       <c r="D13">
-        <v>0.5948816054844092</v>
+        <v>0.606460004449629</v>
       </c>
       <c r="E13">
-        <v>0.794537999950202</v>
+        <v>0.6498446387983596</v>
       </c>
       <c r="F13">
-        <v>0.581515018217733</v>
+        <v>0.6911506500066144</v>
       </c>
       <c r="G13">
-        <v>0.6953903740652518</v>
+        <v>0.5719592197515424</v>
       </c>
       <c r="H13">
-        <v>0.5140762073916688</v>
+        <v>0.564539538561447</v>
       </c>
       <c r="I13">
-        <v>0.5695427722492883</v>
+        <v>0.6448726293699566</v>
       </c>
       <c r="J13">
-        <v>0.6408035721696117</v>
+        <v>0.6568633272401476</v>
       </c>
       <c r="K13">
-        <v>0.5560890386514727</v>
+        <v>0.4899969784613905</v>
       </c>
       <c r="L13">
-        <v>0.5112584760181597</v>
+        <v>0.6499043931066828</v>
       </c>
       <c r="M13">
-        <v>0.4332695954044552</v>
+        <v>0.9125080424037617</v>
       </c>
     </row>
   </sheetData>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0.6480649878884605</v>
@@ -2112,31 +2112,31 @@
         <v>0.4747735159637625</v>
       </c>
       <c r="E2">
-        <v>0.5381304817717157</v>
+        <v>0.6192892042031992</v>
       </c>
       <c r="F2">
-        <v>0.6192892042031992</v>
+        <v>0.6578040931973675</v>
       </c>
       <c r="G2">
-        <v>0.6578040931973675</v>
+        <v>0.4383533366433769</v>
       </c>
       <c r="H2">
-        <v>0.4383533366433769</v>
+        <v>0.886302287760932</v>
       </c>
       <c r="I2">
-        <v>0.886302287760932</v>
+        <v>0.6190238073438649</v>
       </c>
       <c r="J2">
-        <v>0.6190238073438649</v>
+        <v>0.5163254498201096</v>
       </c>
       <c r="K2">
-        <v>0.5163254498201096</v>
+        <v>0.5432955256233967</v>
       </c>
       <c r="L2">
-        <v>0.5432955256233967</v>
+        <v>0.5027758323429803</v>
       </c>
       <c r="M2">
-        <v>0.5027758323429803</v>
+        <v>0.5291997212692967</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2153,36 +2153,36 @@
         <v>0.4189030032339082</v>
       </c>
       <c r="E3">
-        <v>0.5699860102013203</v>
+        <v>0.634470802919708</v>
       </c>
       <c r="F3">
-        <v>0.634470802919708</v>
+        <v>0.559236847725493</v>
       </c>
       <c r="G3">
-        <v>0.559236847725493</v>
+        <v>0.5822674651473847</v>
       </c>
       <c r="H3">
-        <v>0.5822674651473847</v>
+        <v>0.4529419338225827</v>
       </c>
       <c r="I3">
-        <v>0.4529419338225827</v>
+        <v>0.677017048974802</v>
       </c>
       <c r="J3">
-        <v>0.677017048974802</v>
+        <v>0.5018571533532409</v>
       </c>
       <c r="K3">
-        <v>0.5018571533532409</v>
+        <v>0.521347302016447</v>
       </c>
       <c r="L3">
-        <v>0.521347302016447</v>
+        <v>0.6556178547749867</v>
       </c>
       <c r="M3">
-        <v>0.6556178547749867</v>
+        <v>0.5353468883457334</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.623113797907762</v>
@@ -2194,36 +2194,36 @@
         <v>0.7101055899982522</v>
       </c>
       <c r="E4">
-        <v>0.6766226453726454</v>
+        <v>0.6532177228422962</v>
       </c>
       <c r="F4">
-        <v>0.6532177228422962</v>
+        <v>0.7059435557289634</v>
       </c>
       <c r="G4">
-        <v>0.7059435557289634</v>
+        <v>0.5009204666387584</v>
       </c>
       <c r="H4">
-        <v>0.5009204666387584</v>
+        <v>0.5435099719290504</v>
       </c>
       <c r="I4">
-        <v>0.5435099719290504</v>
+        <v>0.8950747353019901</v>
       </c>
       <c r="J4">
-        <v>0.8950747353019901</v>
+        <v>0.3384673272293992</v>
       </c>
       <c r="K4">
-        <v>0.3384673272293992</v>
+        <v>0.5715879980723869</v>
       </c>
       <c r="L4">
-        <v>0.5715879980723869</v>
+        <v>0.6206690539723331</v>
       </c>
       <c r="M4">
-        <v>0.6206690539723331</v>
+        <v>0.7295776622875823</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0.5158985503405507</v>
@@ -2235,36 +2235,36 @@
         <v>0.7175794200344119</v>
       </c>
       <c r="E5">
-        <v>0.6273969123596321</v>
+        <v>0.6433976261127597</v>
       </c>
       <c r="F5">
-        <v>0.6433976261127597</v>
+        <v>0.8941786129407207</v>
       </c>
       <c r="G5">
-        <v>0.8941786129407207</v>
+        <v>0.5512843743798159</v>
       </c>
       <c r="H5">
-        <v>0.5512843743798159</v>
+        <v>0.6059861395940881</v>
       </c>
       <c r="I5">
-        <v>0.6059861395940881</v>
+        <v>0.7738727903334079</v>
       </c>
       <c r="J5">
-        <v>0.7738727903334079</v>
+        <v>0.2519090933483592</v>
       </c>
       <c r="K5">
-        <v>0.2519090933483592</v>
+        <v>0.604443244616655</v>
       </c>
       <c r="L5">
-        <v>0.604443244616655</v>
+        <v>0.5098906100157665</v>
       </c>
       <c r="M5">
-        <v>0.5098906100157665</v>
+        <v>0.6335630172445222</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>0.5940762113862558</v>
@@ -2276,36 +2276,36 @@
         <v>0.5663764345111164</v>
       </c>
       <c r="E6">
-        <v>0.4402233378513725</v>
+        <v>0.6108399034625633</v>
       </c>
       <c r="F6">
-        <v>0.6108399034625633</v>
+        <v>0.5677222303832454</v>
       </c>
       <c r="G6">
-        <v>0.5677222303832454</v>
+        <v>0.9294555025687101</v>
       </c>
       <c r="H6">
-        <v>0.9294555025687101</v>
+        <v>0.5679967826980651</v>
       </c>
       <c r="I6">
-        <v>0.5679967826980651</v>
+        <v>0.3881041885734314</v>
       </c>
       <c r="J6">
-        <v>0.3881041885734314</v>
+        <v>0.3710010586757373</v>
       </c>
       <c r="K6">
-        <v>0.3710010586757373</v>
+        <v>0.5004028402334685</v>
       </c>
       <c r="L6">
-        <v>0.5004028402334685</v>
+        <v>0.5903734094235649</v>
       </c>
       <c r="M6">
-        <v>0.5903734094235649</v>
+        <v>0.6136761556623601</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0.6086267605633804</v>
@@ -2317,36 +2317,36 @@
         <v>0.5420889007088947</v>
       </c>
       <c r="E7">
-        <v>0.52796875</v>
+        <v>0.8111512292634693</v>
       </c>
       <c r="F7">
-        <v>0.8111512292634693</v>
+        <v>0.6202337900091535</v>
       </c>
       <c r="G7">
-        <v>0.6202337900091535</v>
+        <v>0.5159700866648029</v>
       </c>
       <c r="H7">
-        <v>0.5159700866648029</v>
+        <v>0.4931554931554932</v>
       </c>
       <c r="I7">
-        <v>0.4931554931554932</v>
+        <v>0.446596274182481</v>
       </c>
       <c r="J7">
-        <v>0.446596274182481</v>
+        <v>0.476006270886154</v>
       </c>
       <c r="K7">
-        <v>0.476006270886154</v>
+        <v>0.447491916295528</v>
       </c>
       <c r="L7">
-        <v>0.447491916295528</v>
+        <v>0.584965847231372</v>
       </c>
       <c r="M7">
-        <v>0.584965847231372</v>
+        <v>0.5801232933964893</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0.5368825909542522</v>
@@ -2358,31 +2358,31 @@
         <v>0.4744869117799749</v>
       </c>
       <c r="E8">
-        <v>0.5493386654817448</v>
+        <v>0.5767331781156937</v>
       </c>
       <c r="F8">
-        <v>0.5767331781156937</v>
+        <v>0.5075304891871061</v>
       </c>
       <c r="G8">
-        <v>0.5075304891871061</v>
+        <v>0.5290740570285307</v>
       </c>
       <c r="H8">
-        <v>0.5290740570285307</v>
+        <v>0.4132322190484249</v>
       </c>
       <c r="I8">
-        <v>0.4132322190484249</v>
+        <v>0.6089358456873942</v>
       </c>
       <c r="J8">
-        <v>0.6089358456873942</v>
+        <v>0.8178916006730577</v>
       </c>
       <c r="K8">
-        <v>0.8178916006730577</v>
+        <v>0.4015198306246178</v>
       </c>
       <c r="L8">
-        <v>0.4015198306246178</v>
+        <v>0.5130386273970089</v>
       </c>
       <c r="M8">
-        <v>0.5130386273970089</v>
+        <v>0.614549392451782</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2399,31 +2399,31 @@
         <v>0.7172378835731275</v>
       </c>
       <c r="E9">
-        <v>0.5069182389937107</v>
+        <v>0.4243684042212984</v>
       </c>
       <c r="F9">
-        <v>0.4243684042212984</v>
+        <v>0.3291055271048372</v>
       </c>
       <c r="G9">
-        <v>0.3291055271048372</v>
+        <v>0.4805027910525682</v>
       </c>
       <c r="H9">
-        <v>0.4805027910525682</v>
+        <v>0.5851761343180999</v>
       </c>
       <c r="I9">
-        <v>0.5851761343180999</v>
+        <v>0.5504557356401844</v>
       </c>
       <c r="J9">
-        <v>0.5504557356401844</v>
+        <v>0.2316864026133116</v>
       </c>
       <c r="K9">
-        <v>0.2316864026133116</v>
+        <v>0.5095033378770403</v>
       </c>
       <c r="L9">
-        <v>0.5095033378770403</v>
+        <v>0.6135211267605634</v>
       </c>
       <c r="M9">
-        <v>0.6135211267605634</v>
+        <v>0.6111111111111112</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2440,36 +2440,36 @@
         <v>0.6134384274801732</v>
       </c>
       <c r="E10">
-        <v>0.5806773200410497</v>
+        <v>0.4791774891774893</v>
       </c>
       <c r="F10">
-        <v>0.4791774891774893</v>
+        <v>0.6430817610062893</v>
       </c>
       <c r="G10">
-        <v>0.6430817610062893</v>
+        <v>0.4836914440572978</v>
       </c>
       <c r="H10">
-        <v>0.4836914440572978</v>
+        <v>0.5617760617760618</v>
       </c>
       <c r="I10">
-        <v>0.5617760617760618</v>
+        <v>0.5183730588660167</v>
       </c>
       <c r="J10">
-        <v>0.5183730588660167</v>
+        <v>0.3491896319700427</v>
       </c>
       <c r="K10">
-        <v>0.3491896319700427</v>
+        <v>0.5656333716035209</v>
       </c>
       <c r="L10">
-        <v>0.5656333716035209</v>
+        <v>0.5353849117484167</v>
       </c>
       <c r="M10">
-        <v>0.5353849117484167</v>
+        <v>0.577123695976155</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.6989061681263566</v>
@@ -2481,36 +2481,36 @@
         <v>0.5440703719908108</v>
       </c>
       <c r="E11">
-        <v>0.5569154007761699</v>
+        <v>0.6033665553009047</v>
       </c>
       <c r="F11">
-        <v>0.6033665553009047</v>
+        <v>0.64099068233861</v>
       </c>
       <c r="G11">
-        <v>0.64099068233861</v>
+        <v>0.4435060950537389</v>
       </c>
       <c r="H11">
-        <v>0.4435060950537389</v>
+        <v>0.5829276629560938</v>
       </c>
       <c r="I11">
-        <v>0.5829276629560938</v>
+        <v>0.4720304086157744</v>
       </c>
       <c r="J11">
-        <v>0.4720304086157744</v>
+        <v>0.4458492272850917</v>
       </c>
       <c r="K11">
-        <v>0.4458492272850917</v>
+        <v>0.5265733414485697</v>
       </c>
       <c r="L11">
-        <v>0.5265733414485697</v>
+        <v>0.7467689980075931</v>
       </c>
       <c r="M11">
-        <v>0.7467689980075931</v>
+        <v>0.6193391488362838</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.5571916396424818</v>
@@ -2522,72 +2522,72 @@
         <v>0.553680759632412</v>
       </c>
       <c r="E12">
-        <v>0.5200272148411028</v>
+        <v>0.5199710117748938</v>
       </c>
       <c r="F12">
-        <v>0.5199710117748938</v>
+        <v>0.5174017629307777</v>
       </c>
       <c r="G12">
-        <v>0.5174017629307777</v>
+        <v>0.3069351180409627</v>
       </c>
       <c r="H12">
-        <v>0.3069351180409627</v>
+        <v>0.5049457447232601</v>
       </c>
       <c r="I12">
-        <v>0.5049457447232601</v>
+        <v>0.4064436350751809</v>
       </c>
       <c r="J12">
-        <v>0.4064436350751809</v>
+        <v>0.3314616194616195</v>
       </c>
       <c r="K12">
-        <v>0.3314616194616195</v>
+        <v>0.7304194179433181</v>
       </c>
       <c r="L12">
-        <v>0.7304194179433181</v>
+        <v>0.5692436357058248</v>
       </c>
       <c r="M12">
-        <v>0.5692436357058248</v>
+        <v>0.4357175555975352</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.559846061111884</v>
+        <v>0.6680747956224634</v>
       </c>
       <c r="C13">
-        <v>0.4857475276323444</v>
+        <v>0.4193533060856753</v>
       </c>
       <c r="D13">
-        <v>0.549503128450497</v>
+        <v>0.6100628296268495</v>
       </c>
       <c r="E13">
-        <v>0.7517485065487902</v>
+        <v>0.6036714998214026</v>
       </c>
       <c r="F13">
-        <v>0.3978886935548251</v>
+        <v>0.6968244794160874</v>
       </c>
       <c r="G13">
-        <v>0.5552305343154175</v>
+        <v>0.4617065912467584</v>
       </c>
       <c r="H13">
-        <v>0.2574301430905008</v>
+        <v>0.5627266927202736</v>
       </c>
       <c r="I13">
-        <v>0.5143216897821956</v>
+        <v>0.5578392934804595</v>
       </c>
       <c r="J13">
-        <v>0.3433998261515444</v>
+        <v>0.5802980972680924</v>
       </c>
       <c r="K13">
-        <v>0.3521639829462024</v>
+        <v>0.444360424961404</v>
       </c>
       <c r="L13">
-        <v>0.5017951072889705</v>
+        <v>0.6093935565129867</v>
       </c>
       <c r="M13">
-        <v>0.4003967869618839</v>
+        <v>0.9166406131210783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Arabic sentiment model with max length 128 and batch size of 16
</commit_message>
<xml_diff>
--- a/results/results_sentiment.xlsx
+++ b/results/results_sentiment.xlsx
@@ -49,13 +49,13 @@
     <t>Thai</t>
   </si>
   <si>
-    <t>Arabic</t>
-  </si>
-  <si>
     <t>Korean</t>
   </si>
   <si>
     <t>Hebrew</t>
+  </si>
+  <si>
+    <t>Arabic</t>
   </si>
 </sst>
 </file>
@@ -492,13 +492,13 @@
         <v>0.5415421398684998</v>
       </c>
       <c r="K2">
-        <v>0.6778242677824268</v>
+        <v>0.5523012552301255</v>
       </c>
       <c r="L2">
-        <v>0.5523012552301255</v>
+        <v>0.7489539748953975</v>
       </c>
       <c r="M2">
-        <v>0.7489539748953975</v>
+        <v>0.4614465032875075</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -533,13 +533,13 @@
         <v>0.5420098846787479</v>
       </c>
       <c r="K3">
-        <v>0.5733113673805601</v>
+        <v>0.6677649643053267</v>
       </c>
       <c r="L3">
-        <v>0.6677649643053267</v>
+        <v>0.5826468973091707</v>
       </c>
       <c r="M3">
-        <v>0.5826468973091707</v>
+        <v>0.6123009335529929</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -574,13 +574,13 @@
         <v>0.3477443609022556</v>
       </c>
       <c r="K4">
-        <v>0.7612781954887218</v>
+        <v>0.7246240601503759</v>
       </c>
       <c r="L4">
-        <v>0.7246240601503759</v>
+        <v>0.8909774436090225</v>
       </c>
       <c r="M4">
-        <v>0.8909774436090225</v>
+        <v>0.5996240601503759</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -615,13 +615,13 @@
         <v>0.2700228832951945</v>
       </c>
       <c r="K5">
-        <v>0.7391304347826086</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="L5">
-        <v>0.5263157894736842</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="M5">
-        <v>0.7368421052631579</v>
+        <v>0.5491990846681922</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -656,13 +656,13 @@
         <v>0.4278444202108324</v>
       </c>
       <c r="K6">
-        <v>0.5654307524536533</v>
+        <v>0.5912395492548165</v>
       </c>
       <c r="L6">
-        <v>0.5912395492548165</v>
+        <v>0.6168665939658307</v>
       </c>
       <c r="M6">
-        <v>0.6168665939658307</v>
+        <v>0.4218466012359142</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -697,13 +697,13 @@
         <v>0.5277777777777778</v>
       </c>
       <c r="K7">
-        <v>0.5160818713450293</v>
+        <v>0.5906432748538012</v>
       </c>
       <c r="L7">
-        <v>0.5906432748538012</v>
+        <v>0.5877192982456141</v>
       </c>
       <c r="M7">
-        <v>0.5877192982456141</v>
+        <v>0.5394736842105263</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -738,13 +738,13 @@
         <v>0.827054794520548</v>
       </c>
       <c r="K8">
-        <v>0.4289383561643836</v>
+        <v>0.5136986301369864</v>
       </c>
       <c r="L8">
-        <v>0.5136986301369864</v>
+        <v>0.6228595890410958</v>
       </c>
       <c r="M8">
-        <v>0.6228595890410958</v>
+        <v>0.613013698630137</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -779,13 +779,13 @@
         <v>0.2653061224489796</v>
       </c>
       <c r="K9">
-        <v>0.5433673469387755</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="L9">
         <v>0.6428571428571429</v>
       </c>
       <c r="M9">
-        <v>0.6428571428571429</v>
+        <v>0.5255102040816326</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -820,18 +820,18 @@
         <v>0.3524229074889868</v>
       </c>
       <c r="K10">
-        <v>0.8237885462555066</v>
+        <v>0.6255506607929515</v>
       </c>
       <c r="L10">
-        <v>0.6255506607929515</v>
+        <v>0.73568281938326</v>
       </c>
       <c r="M10">
-        <v>0.73568281938326</v>
+        <v>0.7136563876651982</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0.6997840172786177</v>
@@ -861,18 +861,18 @@
         <v>0.4892008639308855</v>
       </c>
       <c r="K11">
-        <v>0.6144708423326134</v>
+        <v>0.7505399568034558</v>
       </c>
       <c r="L11">
-        <v>0.7505399568034558</v>
+        <v>0.6274298056155507</v>
       </c>
       <c r="M11">
-        <v>0.6274298056155507</v>
+        <v>0.4697624190064795</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0.6229491173416407</v>
@@ -902,18 +902,18 @@
         <v>0.3325025960539979</v>
       </c>
       <c r="K12">
-        <v>0.8496365524402908</v>
+        <v>0.7037383177570093</v>
       </c>
       <c r="L12">
-        <v>0.7037383177570093</v>
+        <v>0.4749740394600208</v>
       </c>
       <c r="M12">
-        <v>0.4749740394600208</v>
+        <v>0.8568016614745587</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0.717049576783555</v>
@@ -943,13 +943,13 @@
         <v>0.5808141878274889</v>
       </c>
       <c r="K13">
-        <v>0.6444981862152358</v>
+        <v>0.6187021362353889</v>
       </c>
       <c r="L13">
-        <v>0.6187021362353889</v>
+        <v>0.9286577992744861</v>
       </c>
       <c r="M13">
-        <v>0.9286577992744861</v>
+        <v>0.5368802902055623</v>
       </c>
     </row>
   </sheetData>
@@ -1038,13 +1038,13 @@
         <v>0.5842069837643795</v>
       </c>
       <c r="K2">
-        <v>0.5420116260245246</v>
+        <v>0.5415139052263731</v>
       </c>
       <c r="L2">
-        <v>0.5415139052263731</v>
+        <v>0.5481625933541061</v>
       </c>
       <c r="M2">
-        <v>0.5481625933541061</v>
+        <v>0.54570153832858</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1079,13 +1079,13 @@
         <v>0.56114296873613</v>
       </c>
       <c r="K3">
-        <v>0.6310486977962706</v>
+        <v>0.6959676126342793</v>
       </c>
       <c r="L3">
-        <v>0.6959676126342793</v>
+        <v>0.6408034241092578</v>
       </c>
       <c r="M3">
-        <v>0.6408034241092578</v>
+        <v>0.6138363404454956</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1120,13 +1120,13 @@
         <v>0.5580788721257094</v>
       </c>
       <c r="K4">
-        <v>0.5656575288041319</v>
+        <v>0.624845373577437</v>
       </c>
       <c r="L4">
-        <v>0.624845373577437</v>
+        <v>0.7481069737103315</v>
       </c>
       <c r="M4">
-        <v>0.7481069737103315</v>
+        <v>0.5807045820861156</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1161,13 +1161,13 @@
         <v>0.5601205029689138</v>
       </c>
       <c r="K5">
-        <v>0.6093553302855629</v>
+        <v>0.5840190700104493</v>
       </c>
       <c r="L5">
-        <v>0.5840190700104493</v>
+        <v>0.6286781159095994</v>
       </c>
       <c r="M5">
-        <v>0.6286781159095994</v>
+        <v>0.56019509125236</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1202,13 +1202,13 @@
         <v>0.5370569392096878</v>
       </c>
       <c r="K6">
-        <v>0.5160115499254844</v>
+        <v>0.6350509246071655</v>
       </c>
       <c r="L6">
-        <v>0.6350509246071655</v>
+        <v>0.6198502424881566</v>
       </c>
       <c r="M6">
-        <v>0.6198502424881566</v>
+        <v>0.485006341685441</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1243,13 +1243,13 @@
         <v>0.5637389950290471</v>
       </c>
       <c r="K7">
-        <v>0.5132562559391827</v>
+        <v>0.6009005621635501</v>
       </c>
       <c r="L7">
-        <v>0.6009005621635501</v>
+        <v>0.5898160345219169</v>
       </c>
       <c r="M7">
-        <v>0.5898160345219169</v>
+        <v>0.5487488556606652</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1284,13 +1284,13 @@
         <v>0.8254863278063406</v>
       </c>
       <c r="K8">
-        <v>0.4764577684147344</v>
+        <v>0.5400789715637987</v>
       </c>
       <c r="L8">
-        <v>0.5400789715637987</v>
+        <v>0.6141441120607787</v>
       </c>
       <c r="M8">
-        <v>0.6141441120607787</v>
+        <v>0.6329818797262812</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1325,13 +1325,13 @@
         <v>0.4674202127659575</v>
       </c>
       <c r="K9">
-        <v>0.5370138834622697</v>
+        <v>0.6304415909802693</v>
       </c>
       <c r="L9">
-        <v>0.6304415909802693</v>
+        <v>0.6256410256410256</v>
       </c>
       <c r="M9">
-        <v>0.6256410256410256</v>
+        <v>0.551557239057239</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1366,18 +1366,18 @@
         <v>0.5614973262032086</v>
       </c>
       <c r="K10">
-        <v>0.6074229691876751</v>
+        <v>0.5622785829307568</v>
       </c>
       <c r="L10">
-        <v>0.5622785829307568</v>
+        <v>0.5717306441119063</v>
       </c>
       <c r="M10">
-        <v>0.5717306441119063</v>
+        <v>0.5835686053077358</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0.7050394725143079</v>
@@ -1407,18 +1407,18 @@
         <v>0.6019638941102756</v>
       </c>
       <c r="K11">
-        <v>0.6114594692838967</v>
+        <v>0.7455492957746479</v>
       </c>
       <c r="L11">
-        <v>0.7455492957746479</v>
+        <v>0.618901976404537</v>
       </c>
       <c r="M11">
-        <v>0.618901976404537</v>
+        <v>0.6192671394799054</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0.5878673226891276</v>
@@ -1448,18 +1448,18 @@
         <v>0.5381076898969719</v>
       </c>
       <c r="K12">
-        <v>0.7323922670754557</v>
+        <v>0.5667899878492364</v>
       </c>
       <c r="L12">
-        <v>0.5667899878492364</v>
+        <v>0.5196306690911008</v>
       </c>
       <c r="M12">
-        <v>0.5196306690911008</v>
+        <v>0.7455789338049237</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0.6707604416216316</v>
@@ -1489,13 +1489,13 @@
         <v>0.6488247962290792</v>
       </c>
       <c r="K13">
-        <v>0.4718507817523435</v>
+        <v>0.6300606871617893</v>
       </c>
       <c r="L13">
-        <v>0.6300606871617893</v>
+        <v>0.9211556022806627</v>
       </c>
       <c r="M13">
-        <v>0.9211556022806627</v>
+        <v>0.6150117178484136</v>
       </c>
     </row>
   </sheetData>
@@ -1584,13 +1584,13 @@
         <v>0.6278099888109043</v>
       </c>
       <c r="K2">
-        <v>0.5493503248375812</v>
+        <v>0.5641493412585743</v>
       </c>
       <c r="L2">
-        <v>0.5641493412585743</v>
+        <v>0.5301464312091742</v>
       </c>
       <c r="M2">
-        <v>0.5301464312091742</v>
+        <v>0.5654838509948565</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1625,13 +1625,13 @@
         <v>0.5415436280470152</v>
       </c>
       <c r="K3">
-        <v>0.5738557408372416</v>
+        <v>0.6680761826182618</v>
       </c>
       <c r="L3">
-        <v>0.6680761826182618</v>
+        <v>0.5831741068843727</v>
       </c>
       <c r="M3">
-        <v>0.5831741068843727</v>
+        <v>0.6123939696601239</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1666,13 +1666,13 @@
         <v>0.5985534637506852</v>
       </c>
       <c r="K4">
-        <v>0.601408900125181</v>
+        <v>0.7642383184834278</v>
       </c>
       <c r="L4">
-        <v>0.7642383184834278</v>
+        <v>0.7147345425983653</v>
       </c>
       <c r="M4">
-        <v>0.7147345425983653</v>
+        <v>0.6864010865385402</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1707,13 +1707,13 @@
         <v>0.5210318914956011</v>
       </c>
       <c r="K5">
-        <v>0.6008369990224829</v>
+        <v>0.6178977272727273</v>
       </c>
       <c r="L5">
-        <v>0.6178977272727273</v>
+        <v>0.640533357771261</v>
       </c>
       <c r="M5">
-        <v>0.640533357771261</v>
+        <v>0.5876557917888563</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1748,13 +1748,13 @@
         <v>0.5132895950581968</v>
       </c>
       <c r="K6">
-        <v>0.512352849724822</v>
+        <v>0.6284168195433393</v>
       </c>
       <c r="L6">
-        <v>0.6284168195433393</v>
+        <v>0.6252496294684038</v>
       </c>
       <c r="M6">
-        <v>0.6252496294684038</v>
+        <v>0.4912958759574226</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1789,13 +1789,13 @@
         <v>0.5364210364210364</v>
       </c>
       <c r="K7">
-        <v>0.5071610071610072</v>
+        <v>0.5941325941325941</v>
       </c>
       <c r="L7">
-        <v>0.5941325941325941</v>
+        <v>0.5845845845845846</v>
       </c>
       <c r="M7">
-        <v>0.5845845845845846</v>
+        <v>0.5437360437360437</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1830,13 +1830,13 @@
         <v>0.8133223166330172</v>
       </c>
       <c r="K8">
-        <v>0.4847636454959374</v>
+        <v>0.5387295438008679</v>
       </c>
       <c r="L8">
-        <v>0.5387295438008679</v>
+        <v>0.6167284648926137</v>
       </c>
       <c r="M8">
-        <v>0.6167284648926137</v>
+        <v>0.5345170975091788</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1871,13 +1871,13 @@
         <v>0.4931972789115647</v>
       </c>
       <c r="K9">
-        <v>0.5493197278911565</v>
+        <v>0.6734693877551021</v>
       </c>
       <c r="L9">
-        <v>0.6734693877551021</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="M9">
-        <v>0.6666666666666667</v>
+        <v>0.5680272108843537</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1912,18 +1912,18 @@
         <v>0.5821428571428571</v>
       </c>
       <c r="K10">
-        <v>0.5570684523809524</v>
+        <v>0.6151041666666667</v>
       </c>
       <c r="L10">
-        <v>0.6151041666666667</v>
+        <v>0.5984375</v>
       </c>
       <c r="M10">
-        <v>0.5984375</v>
+        <v>0.6321428571428571</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0.7100525904512616</v>
@@ -1953,18 +1953,18 @@
         <v>0.5499297675377409</v>
       </c>
       <c r="K11">
-        <v>0.5587987132837631</v>
+        <v>0.7507370813018653</v>
       </c>
       <c r="L11">
-        <v>0.7507370813018653</v>
+        <v>0.6202101700440571</v>
       </c>
       <c r="M11">
-        <v>0.6202101700440571</v>
+        <v>0.538697367601022</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0.654357745398773</v>
@@ -1994,18 +1994,18 @@
         <v>0.5447595858895705</v>
       </c>
       <c r="K12">
-        <v>0.7285118865030675</v>
+        <v>0.5940479294478528</v>
       </c>
       <c r="L12">
-        <v>0.5940479294478528</v>
+        <v>0.5342756901840491</v>
       </c>
       <c r="M12">
-        <v>0.5342756901840491</v>
+        <v>0.7521200153374233</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0.6658678129472178</v>
@@ -2035,13 +2035,13 @@
         <v>0.6568633272401476</v>
       </c>
       <c r="K13">
-        <v>0.4899969784613905</v>
+        <v>0.6499043931066828</v>
       </c>
       <c r="L13">
-        <v>0.6499043931066828</v>
+        <v>0.9125080424037617</v>
       </c>
       <c r="M13">
-        <v>0.9125080424037617</v>
+        <v>0.6168561266580881</v>
       </c>
     </row>
   </sheetData>
@@ -2130,13 +2130,13 @@
         <v>0.5163254498201096</v>
       </c>
       <c r="K2">
-        <v>0.5432955256233967</v>
+        <v>0.5027758323429803</v>
       </c>
       <c r="L2">
-        <v>0.5027758323429803</v>
+        <v>0.5291997212692967</v>
       </c>
       <c r="M2">
-        <v>0.5291997212692967</v>
+        <v>0.4470444004814329</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2171,13 +2171,13 @@
         <v>0.5018571533532409</v>
       </c>
       <c r="K3">
-        <v>0.521347302016447</v>
+        <v>0.6556178547749867</v>
       </c>
       <c r="L3">
-        <v>0.6556178547749867</v>
+        <v>0.5353468883457334</v>
       </c>
       <c r="M3">
-        <v>0.5353468883457334</v>
+        <v>0.6111045906637951</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2212,13 +2212,13 @@
         <v>0.3384673272293992</v>
       </c>
       <c r="K4">
-        <v>0.5715879980723869</v>
+        <v>0.6206690539723331</v>
       </c>
       <c r="L4">
-        <v>0.6206690539723331</v>
+        <v>0.7295776622875823</v>
       </c>
       <c r="M4">
-        <v>0.7295776622875823</v>
+        <v>0.5223329455207648</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2253,13 +2253,13 @@
         <v>0.2519090933483592</v>
       </c>
       <c r="K5">
-        <v>0.604443244616655</v>
+        <v>0.5098906100157665</v>
       </c>
       <c r="L5">
-        <v>0.5098906100157665</v>
+        <v>0.6335630172445222</v>
       </c>
       <c r="M5">
-        <v>0.6335630172445222</v>
+        <v>0.5162805594106972</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2294,13 +2294,13 @@
         <v>0.3710010586757373</v>
       </c>
       <c r="K6">
-        <v>0.5004028402334685</v>
+        <v>0.5903734094235649</v>
       </c>
       <c r="L6">
-        <v>0.5903734094235649</v>
+        <v>0.6136761556623601</v>
       </c>
       <c r="M6">
-        <v>0.6136761556623601</v>
+        <v>0.3899010360922989</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2335,13 +2335,13 @@
         <v>0.476006270886154</v>
       </c>
       <c r="K7">
-        <v>0.447491916295528</v>
+        <v>0.584965847231372</v>
       </c>
       <c r="L7">
-        <v>0.584965847231372</v>
+        <v>0.5801232933964893</v>
       </c>
       <c r="M7">
-        <v>0.5801232933964893</v>
+        <v>0.5292086833968819</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2376,13 +2376,13 @@
         <v>0.8178916006730577</v>
       </c>
       <c r="K8">
-        <v>0.4015198306246178</v>
+        <v>0.5130386273970089</v>
       </c>
       <c r="L8">
-        <v>0.5130386273970089</v>
+        <v>0.614549392451782</v>
       </c>
       <c r="M8">
-        <v>0.614549392451782</v>
+        <v>0.4658977899853812</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2417,13 +2417,13 @@
         <v>0.2316864026133116</v>
       </c>
       <c r="K9">
-        <v>0.5095033378770403</v>
+        <v>0.6135211267605634</v>
       </c>
       <c r="L9">
-        <v>0.6135211267605634</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="M9">
-        <v>0.6111111111111112</v>
+        <v>0.5059493156254234</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2458,18 +2458,18 @@
         <v>0.3491896319700427</v>
       </c>
       <c r="K10">
-        <v>0.5656333716035209</v>
+        <v>0.5353849117484167</v>
       </c>
       <c r="L10">
-        <v>0.5353849117484167</v>
+        <v>0.577123695976155</v>
       </c>
       <c r="M10">
-        <v>0.577123695976155</v>
+        <v>0.586149833113623</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0.6989061681263566</v>
@@ -2499,18 +2499,18 @@
         <v>0.4458492272850917</v>
       </c>
       <c r="K11">
-        <v>0.5265733414485697</v>
+        <v>0.7467689980075931</v>
       </c>
       <c r="L11">
-        <v>0.7467689980075931</v>
+        <v>0.6193391488362838</v>
       </c>
       <c r="M11">
-        <v>0.6193391488362838</v>
+        <v>0.404284701668049</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0.5571916396424818</v>
@@ -2540,18 +2540,18 @@
         <v>0.3314616194616195</v>
       </c>
       <c r="K12">
-        <v>0.7304194179433181</v>
+        <v>0.5692436357058248</v>
       </c>
       <c r="L12">
-        <v>0.5692436357058248</v>
+        <v>0.4357175555975352</v>
       </c>
       <c r="M12">
-        <v>0.4357175555975352</v>
+        <v>0.7487636374471636</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0.6680747956224634</v>
@@ -2581,13 +2581,13 @@
         <v>0.5802980972680924</v>
       </c>
       <c r="K13">
-        <v>0.444360424961404</v>
+        <v>0.6093935565129867</v>
       </c>
       <c r="L13">
-        <v>0.6093935565129867</v>
+        <v>0.9166406131210783</v>
       </c>
       <c r="M13">
-        <v>0.9166406131210783</v>
+        <v>0.5368369488129967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>